<commit_message>
Atualização dos documentos para a primeira sprint
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\TCC - BPM Game Engine\Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82D8A358-7B7E-4FF7-B9B0-794AE60B8DE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC245D8-9E8A-47C4-B2D6-D076FD65B6B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -30,9 +30,251 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
+  <si>
+    <t>BPM Game Engine</t>
+  </si>
+  <si>
+    <t>Informações do documento</t>
+  </si>
+  <si>
+    <t>Nome do Projeto:</t>
+  </si>
+  <si>
+    <t>Documentado por:</t>
+  </si>
+  <si>
+    <t>Revisado por:</t>
+  </si>
+  <si>
+    <t>Versão do documento:</t>
+  </si>
+  <si>
+    <t>Data:</t>
+  </si>
+  <si>
+    <t>Data da Revisão:</t>
+  </si>
+  <si>
+    <t>Lista de Requisitos</t>
+  </si>
+  <si>
+    <t>ID#</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Prioridade</t>
+  </si>
+  <si>
+    <t>Componente</t>
+  </si>
+  <si>
+    <t>Dependência</t>
+  </si>
+  <si>
+    <t>PROJETO</t>
+  </si>
+  <si>
+    <t>BPM GAME ENGINE</t>
+  </si>
+  <si>
+    <t>Fabio Takeshi Ishikawa</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Sprint</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#6</t>
+  </si>
+  <si>
+    <t>#7</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>#14</t>
+  </si>
+  <si>
+    <t>#15</t>
+  </si>
+  <si>
+    <t>#16</t>
+  </si>
+  <si>
+    <t>#17</t>
+  </si>
+  <si>
+    <t>#18</t>
+  </si>
+  <si>
+    <t>#19</t>
+  </si>
+  <si>
+    <t>#20</t>
+  </si>
+  <si>
+    <t>Sistema de Janelas</t>
+  </si>
+  <si>
+    <t>Criar uma janela de aplicação</t>
+  </si>
+  <si>
+    <t>Destruir uma janela de aplicação</t>
+  </si>
+  <si>
+    <t>Destruir uma janela de aplicação previamente criada utilizando a classe Window.</t>
+  </si>
+  <si>
+    <t>Criar uma janela de aplicação utilizando a classe Window.</t>
+  </si>
+  <si>
+    <t>Nenhuma</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Finalizada</t>
+  </si>
+  <si>
+    <t>18/02/2020</t>
+  </si>
+  <si>
+    <t>Customizar uma janela de aplicação</t>
+  </si>
+  <si>
+    <t>Alguns estilos de janelas são dependentes do Sistema Operacional utilizado.</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>27/02/2020</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe Engine e realizar a inicialização do objeto (configuração de valores padrão para a Engine e configuração de valores padrão relacionada ao Sistema Operacional).</t>
+  </si>
+  <si>
+    <t>Core Engine</t>
+  </si>
+  <si>
+    <t>20/02/2020</t>
+  </si>
+  <si>
+    <t>Personalizar uma janela de aplicação antes de sua criação. Tipos possíveis de personalização: posicionamento inicial da janela, diferentes tipos de tamanho, diferente estilos*, texto do título da janela, tela cheia ou popup. (*) Consulte o documento "Guia de Desenvolvimento" para obter mais detalhes sobres todos os estilos possíveis de janela que podem ser criados.</t>
+  </si>
+  <si>
+    <t>25/02/2020</t>
+  </si>
+  <si>
+    <t>Iniciar o processamento principal (main loop) da game engine.</t>
+  </si>
+  <si>
+    <t>Executar a game engine</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto Game Engine</t>
+  </si>
+  <si>
+    <t>Configurar as funções de eventos globais da game engine</t>
+  </si>
+  <si>
+    <t>Definir as funções de eventos globais do usuário e configurar na game engine.</t>
+  </si>
+  <si>
+    <t>Realizar todas as ações com o mouse, incluindo movimentação e "cliques" dos três botões do mouse.</t>
+  </si>
+  <si>
+    <t>Sistema de Entrada e Saída</t>
+  </si>
+  <si>
+    <t>21/02/2020</t>
+  </si>
+  <si>
+    <t>Realizar entrada de dados com o mouse</t>
+  </si>
+  <si>
+    <t>Realizar entrada de dados com o teclado</t>
+  </si>
+  <si>
+    <t>Realizar todas as ações com o teclado, incluindo todos os caracteres ASCII e todos os caracteres especiais como, por exemplo, CTRL, SHIFT, F1 e HOME.</t>
+  </si>
+  <si>
+    <t>23/02/2020</t>
+  </si>
+  <si>
+    <t>Definir diferentes modos de renderização</t>
+  </si>
+  <si>
+    <t>Configurar diferentes modos de renderização como o formato do pixel, double buffering, buffer de pronfudidade.</t>
+  </si>
+  <si>
+    <t>Sistema de Renderização</t>
+  </si>
+  <si>
+    <t>24/02/2020</t>
+  </si>
+  <si>
+    <t>Customizar o ícone da janela de aplicação utilizando recurso externo.</t>
+  </si>
+  <si>
+    <t>Gerenciador de Assets</t>
+  </si>
+  <si>
+    <t>Customizar o ícone da janela de aplicação</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,16 +282,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -57,12 +335,555 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,12 +1198,653 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27:D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="63"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="65"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="34"/>
+      <c r="C5" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="34"/>
+      <c r="I5" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="38"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="36"/>
+      <c r="I6" s="39">
+        <v>44046</v>
+      </c>
+      <c r="J6" s="40"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="32"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="42"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="82" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="73" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="30"/>
+      <c r="E18" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="82" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="30"/>
+      <c r="E19" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="82" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="82" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="79">
+        <v>43864</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="70"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="77"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="70"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="77"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="70"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="77"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="70"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="77"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="70"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="77"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="70"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="77"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="70"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="77"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="70"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="77"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" s="70"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="77"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="70"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="77"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="77"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="78"/>
+    </row>
+  </sheetData>
+  <mergeCells count="38">
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="I1:J2"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inclusão da classe GEWinApiWrapper
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC245D8-9E8A-47C4-B2D6-D076FD65B6B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8A008D-E029-43F6-8909-7E1CE887CC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
   <si>
     <t>BPM Game Engine</t>
   </si>
@@ -63,21 +63,6 @@
     <t>ID#</t>
   </si>
   <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Prioridade</t>
-  </si>
-  <si>
-    <t>Componente</t>
-  </si>
-  <si>
-    <t>Dependência</t>
-  </si>
-  <si>
     <t>PROJETO</t>
   </si>
   <si>
@@ -90,15 +75,6 @@
     <t>1.0.0</t>
   </si>
   <si>
-    <t>Sprint</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Nome</t>
-  </si>
-  <si>
     <t>#1</t>
   </si>
   <si>
@@ -129,9 +105,6 @@
     <t>#11</t>
   </si>
   <si>
-    <t>#12</t>
-  </si>
-  <si>
     <t>#13</t>
   </si>
   <si>
@@ -168,9 +141,6 @@
     <t>Destruir uma janela de aplicação previamente criada utilizando a classe Window.</t>
   </si>
   <si>
-    <t>Criar uma janela de aplicação utilizando a classe Window.</t>
-  </si>
-  <si>
     <t>Nenhuma</t>
   </si>
   <si>
@@ -265,6 +235,39 @@
   </si>
   <si>
     <t>Customizar o ícone da janela de aplicação</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>COMPONENTE</t>
+  </si>
+  <si>
+    <t>DEPENDÊNCIA</t>
+  </si>
+  <si>
+    <t>SPRINT</t>
+  </si>
+  <si>
+    <t>PRIORIDADE</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GEWindow e configurar todos os seus atributos.</t>
+  </si>
+  <si>
+    <t>Criar uma janela de aplicação no Microsoft Windows com um objeto GEWindow.</t>
+  </si>
+  <si>
+    <t>ApiWrapper</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +309,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -636,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -698,6 +709,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -710,6 +778,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -722,102 +847,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -833,56 +877,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1200,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,32 +1223,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="58" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="63"/>
+      <c r="A1" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="60"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="65"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1251,60 +1256,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="46" t="s">
+      <c r="B5" s="49"/>
+      <c r="C5" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="33" t="s">
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="38"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="77" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="78"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="35" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="39">
+      <c r="H6" s="51"/>
+      <c r="I6" s="79">
         <v>44046</v>
       </c>
-      <c r="J6" s="40"/>
+      <c r="J6" s="80"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="31" t="s">
+      <c r="B7" s="47"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="42"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1316,495 +1321,511 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="26"/>
+        <v>69</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="64"/>
       <c r="E11" s="2" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="80" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="66" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>36</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="67" t="s">
-        <v>46</v>
+        <v>15</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="45"/>
+      <c r="E13" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="81" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="30"/>
-      <c r="E14" s="73" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="67" t="s">
-        <v>51</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="45"/>
+      <c r="E14" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="20" t="s">
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="39"/>
+      <c r="E17" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="18" t="s">
         <v>48</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="82" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="J16" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="82" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="82" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="76" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="82" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="76" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="67" t="s">
-        <v>46</v>
+        <v>20</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="82" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="F20" s="67" t="s">
-        <v>46</v>
+        <v>21</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="39"/>
+      <c r="E20" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="76" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="67" t="s">
-        <v>46</v>
+        <v>22</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="39"/>
+      <c r="E21" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="79">
+        <v>38</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="39"/>
+      <c r="E22" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" s="34">
         <v>43864</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="77"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="68"/>
+        <v>24</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="23"/>
       <c r="G23" s="8"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="77"/>
+      <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="68"/>
+        <v>25</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="8"/>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
-      <c r="J24" s="77"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="70"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="68"/>
+        <v>26</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="23"/>
       <c r="G25" s="8"/>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="77"/>
+      <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="68"/>
+        <v>27</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="23"/>
       <c r="G26" s="8"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="77"/>
+      <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="70"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="68"/>
+        <v>28</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="8"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
-      <c r="J27" s="77"/>
+      <c r="J27" s="32"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="70"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="74"/>
-      <c r="F28" s="68"/>
+        <v>29</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="23"/>
       <c r="G28" s="8"/>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
-      <c r="J28" s="77"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="68"/>
+        <v>30</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="8"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
-      <c r="J29" s="77"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="68"/>
+        <v>31</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="8"/>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="77"/>
+      <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="74"/>
-      <c r="F31" s="68"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="8"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="77"/>
+      <c r="J31" s="32"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="70"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="74"/>
-      <c r="F32" s="68"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="8"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
-      <c r="J32" s="77"/>
+      <c r="J32" s="32"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
-      <c r="B33" s="71"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="69"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="24"/>
       <c r="G33" s="10"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
-      <c r="J33" s="78"/>
+      <c r="J33" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="30">
     <mergeCell ref="C1:H2"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
@@ -1814,25 +1835,17 @@
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>

</xml_diff>

<commit_message>
Melhorando a bateria de testes para GEWindow
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8A008D-E029-43F6-8909-7E1CE887CC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73B5BA1-3802-4D18-9649-9B24235BF35D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>Destruir uma janela de aplicação</t>
   </si>
   <si>
-    <t>Destruir uma janela de aplicação previamente criada utilizando a classe Window.</t>
-  </si>
-  <si>
     <t>Nenhuma</t>
   </si>
   <si>
@@ -268,6 +265,9 @@
   </si>
   <si>
     <t>ApiWrapper</t>
+  </si>
+  <si>
+    <t>Destruir uma janela de aplicação no Microsoft Windows utilizando a classe Window.</t>
   </si>
 </sst>
 </file>
@@ -766,6 +766,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -777,117 +888,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1206,7 +1206,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,32 +1223,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="67" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="74"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1256,60 +1256,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="57" t="s">
+      <c r="B5" s="74"/>
+      <c r="C5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="48" t="s">
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="49"/>
-      <c r="I5" s="77" t="s">
+      <c r="H5" s="74"/>
+      <c r="I5" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="78"/>
+      <c r="J5" s="51"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="60" t="s">
+      <c r="B6" s="76"/>
+      <c r="C6" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="50" t="s">
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="51"/>
-      <c r="I6" s="79">
+      <c r="H6" s="76"/>
+      <c r="I6" s="52">
         <v>44046</v>
       </c>
-      <c r="J6" s="80"/>
+      <c r="J6" s="53"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="46" t="s">
+      <c r="B7" s="72"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="47"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="55"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1321,29 +1321,29 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="64"/>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1353,27 +1353,27 @@
       <c r="B12" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="65" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="66"/>
+      <c r="C12" s="67" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="68"/>
       <c r="E12" s="27" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="J12" s="14" t="s">
         <v>38</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1383,57 +1383,57 @@
       <c r="B13" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="45"/>
+      <c r="C13" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="70"/>
       <c r="E13" s="28" t="s">
         <v>32</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="J13" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="45"/>
+      <c r="C14" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="70"/>
       <c r="E14" s="28" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="J14" s="18" t="s">
         <v>38</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1441,29 +1441,29 @@
         <v>16</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="28" t="s">
         <v>32</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>42</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1471,29 +1471,29 @@
         <v>17</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="39"/>
       <c r="E16" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="20" t="s">
-        <v>38</v>
-      </c>
       <c r="J16" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1501,29 +1501,29 @@
         <v>18</v>
       </c>
       <c r="B17" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>53</v>
       </c>
       <c r="D17" s="39"/>
       <c r="E17" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1531,29 +1531,29 @@
         <v>19</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I18" s="20" t="s">
-        <v>38</v>
-      </c>
       <c r="J18" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1561,29 +1561,29 @@
         <v>20</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1591,29 +1591,29 @@
         <v>21</v>
       </c>
       <c r="B20" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="38" t="s">
         <v>58</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>59</v>
       </c>
       <c r="D20" s="39"/>
       <c r="E20" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1621,29 +1621,29 @@
         <v>22</v>
       </c>
       <c r="B21" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="38" t="s">
         <v>61</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>62</v>
       </c>
       <c r="D21" s="39"/>
       <c r="E21" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G21" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1651,26 +1651,26 @@
         <v>23</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="39"/>
       <c r="E22" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G22" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J22" s="34">
         <v>43864</v>
@@ -1681,8 +1681,8 @@
         <v>24</v>
       </c>
       <c r="B23" s="25"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="78"/>
       <c r="E23" s="29"/>
       <c r="F23" s="23"/>
       <c r="G23" s="8"/>
@@ -1695,8 +1695,8 @@
         <v>25</v>
       </c>
       <c r="B24" s="25"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="41"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="29"/>
       <c r="F24" s="23"/>
       <c r="G24" s="8"/>
@@ -1709,8 +1709,8 @@
         <v>26</v>
       </c>
       <c r="B25" s="25"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="78"/>
       <c r="E25" s="29"/>
       <c r="F25" s="23"/>
       <c r="G25" s="8"/>
@@ -1723,8 +1723,8 @@
         <v>27</v>
       </c>
       <c r="B26" s="25"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="41"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="78"/>
       <c r="E26" s="29"/>
       <c r="F26" s="23"/>
       <c r="G26" s="8"/>
@@ -1737,8 +1737,8 @@
         <v>28</v>
       </c>
       <c r="B27" s="25"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="41"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="78"/>
       <c r="E27" s="29"/>
       <c r="F27" s="23"/>
       <c r="G27" s="8"/>
@@ -1751,8 +1751,8 @@
         <v>29</v>
       </c>
       <c r="B28" s="25"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="41"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="78"/>
       <c r="E28" s="29"/>
       <c r="F28" s="23"/>
       <c r="G28" s="8"/>
@@ -1765,8 +1765,8 @@
         <v>30</v>
       </c>
       <c r="B29" s="25"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="41"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="78"/>
       <c r="E29" s="29"/>
       <c r="F29" s="23"/>
       <c r="G29" s="8"/>
@@ -1779,8 +1779,8 @@
         <v>31</v>
       </c>
       <c r="B30" s="25"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="41"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="78"/>
       <c r="E30" s="29"/>
       <c r="F30" s="23"/>
       <c r="G30" s="8"/>
@@ -1791,8 +1791,8 @@
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="25"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="41"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="78"/>
       <c r="E31" s="29"/>
       <c r="F31" s="23"/>
       <c r="G31" s="8"/>
@@ -1803,8 +1803,8 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="25"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="41"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="78"/>
       <c r="E32" s="29"/>
       <c r="F32" s="23"/>
       <c r="G32" s="8"/>
@@ -1815,8 +1815,8 @@
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="26"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="80"/>
       <c r="E33" s="30"/>
       <c r="F33" s="24"/>
       <c r="G33" s="10"/>
@@ -1826,16 +1826,17 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C1:H2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="I1:J2"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -1845,17 +1846,16 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="I1:J2"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Inclusão da classe GameEngine
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73B5BA1-3802-4D18-9649-9B24235BF35D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C63AE-58EA-458A-9435-263C5C72D52A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
   <si>
     <t>BPM Game Engine</t>
   </si>
@@ -105,9 +105,6 @@
     <t>#11</t>
   </si>
   <si>
-    <t>#13</t>
-  </si>
-  <si>
     <t>#14</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>27/02/2020</t>
   </si>
   <si>
-    <t>Instanciar um objeto da classe Engine e realizar a inicialização do objeto (configuração de valores padrão para a Engine e configuração de valores padrão relacionada ao Sistema Operacional).</t>
-  </si>
-  <si>
     <t>Core Engine</t>
   </si>
   <si>
@@ -177,21 +171,9 @@
     <t>25/02/2020</t>
   </si>
   <si>
-    <t>Iniciar o processamento principal (main loop) da game engine.</t>
-  </si>
-  <si>
-    <t>Executar a game engine</t>
-  </si>
-  <si>
     <t>Instanciar um objeto Game Engine</t>
   </si>
   <si>
-    <t>Configurar as funções de eventos globais da game engine</t>
-  </si>
-  <si>
-    <t>Definir as funções de eventos globais do usuário e configurar na game engine.</t>
-  </si>
-  <si>
     <t>Realizar todas as ações com o mouse, incluindo movimentação e "cliques" dos três botões do mouse.</t>
   </si>
   <si>
@@ -268,6 +250,39 @@
   </si>
   <si>
     <t>Destruir uma janela de aplicação no Microsoft Windows utilizando a classe Window.</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GameEngine passando uma referência a um objeto da classe ApiWrapper no construtor.</t>
+  </si>
+  <si>
+    <t>ApiWrapper WinApiWrapper</t>
+  </si>
+  <si>
+    <t>Definir funções de eventos globais</t>
+  </si>
+  <si>
+    <t>Criar uma nova classe que herde da classe GEEventHandler e definir as funções de eventos globais do usuário.</t>
+  </si>
+  <si>
+    <t>GEEventHandler</t>
+  </si>
+  <si>
+    <t>Iniciar o loop principal da Game Engine</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GameEngine passando uma referência a um objeto da classe ApiWrapper no construtor e executar o loop principal do motor de jogo.</t>
+  </si>
+  <si>
+    <t>Chamar métodos de uma classe herdada de ApiWrapper (polimorfismo)</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe WinApiWrapper, atribui-lo a um ponteiro para ApiWrapper. Então, chamar os métodos definidos em WinApiWrapper através do ponteiro para ApiWrapper.</t>
+  </si>
+  <si>
+    <t>Camada Multiplataforma</t>
+  </si>
+  <si>
+    <t>WinApiWrapper</t>
   </si>
 </sst>
 </file>
@@ -766,6 +781,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -807,87 +903,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -907,7 +922,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1205,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,39 +1231,39 @@
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="8" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="47"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="49"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1256,58 +1271,58 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="74"/>
+      <c r="B5" s="51"/>
       <c r="C5" s="59" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="60"/>
       <c r="E5" s="60"/>
       <c r="F5" s="61"/>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="50" t="s">
+      <c r="H5" s="51"/>
+      <c r="I5" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="51"/>
+      <c r="J5" s="78"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="76"/>
+      <c r="B6" s="53"/>
       <c r="C6" s="62" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="63"/>
       <c r="E6" s="63"/>
       <c r="F6" s="64"/>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="76"/>
-      <c r="I6" s="52">
+      <c r="H6" s="53"/>
+      <c r="I6" s="79">
         <v>44046</v>
       </c>
-      <c r="J6" s="53"/>
+      <c r="J6" s="80"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="72"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="56"/>
       <c r="D7" s="57"/>
       <c r="E7" s="57"/>
       <c r="F7" s="58"/>
-      <c r="G7" s="71" t="s">
+      <c r="G7" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="72"/>
+      <c r="H7" s="49"/>
       <c r="I7" s="54"/>
       <c r="J7" s="55"/>
     </row>
@@ -1321,239 +1336,239 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C11" s="65" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D11" s="66"/>
       <c r="E11" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="68"/>
+        <v>32</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="45"/>
       <c r="E12" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="J12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="70"/>
+        <v>32</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="47"/>
       <c r="E13" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="J13" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="J13" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="69" t="s">
-        <v>78</v>
-      </c>
-      <c r="D14" s="70"/>
+        <v>33</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="47"/>
       <c r="E14" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="20" t="s">
+      <c r="J14" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="C15" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="47"/>
       <c r="E15" s="28" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="39"/>
+        <v>18</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="47"/>
       <c r="E16" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="20" t="s">
         <v>36</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>37</v>
       </c>
       <c r="J16" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="39"/>
+        <v>78</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="47"/>
       <c r="E17" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="28" t="s">
-        <v>44</v>
+        <v>20</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="31" t="s">
+        <v>82</v>
       </c>
       <c r="F18" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="17" t="s">
+      <c r="I18" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>45</v>
+      <c r="J18" s="18">
+        <v>43906</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1561,29 +1576,29 @@
         <v>20</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="31" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1591,29 +1606,29 @@
         <v>21</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D20" s="39"/>
       <c r="E20" s="31" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1621,29 +1636,29 @@
         <v>22</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D21" s="39"/>
       <c r="E21" s="31" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G21" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1651,52 +1666,68 @@
         <v>23</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D22" s="39"/>
       <c r="E22" s="31" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G22" s="16" t="s">
         <v>14</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I22" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J22" s="34">
         <v>43864</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="32"/>
+    <row r="23" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="25"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="78"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41"/>
       <c r="E24" s="29"/>
       <c r="F24" s="23"/>
       <c r="G24" s="8"/>
@@ -1706,11 +1737,11 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="25"/>
-      <c r="C25" s="77"/>
-      <c r="D25" s="78"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41"/>
       <c r="E25" s="29"/>
       <c r="F25" s="23"/>
       <c r="G25" s="8"/>
@@ -1720,11 +1751,11 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="25"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="78"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41"/>
       <c r="E26" s="29"/>
       <c r="F26" s="23"/>
       <c r="G26" s="8"/>
@@ -1734,11 +1765,11 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="25"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="78"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41"/>
       <c r="E27" s="29"/>
       <c r="F27" s="23"/>
       <c r="G27" s="8"/>
@@ -1748,11 +1779,11 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="25"/>
-      <c r="C28" s="77"/>
-      <c r="D28" s="78"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="41"/>
       <c r="E28" s="29"/>
       <c r="F28" s="23"/>
       <c r="G28" s="8"/>
@@ -1762,11 +1793,11 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="25"/>
-      <c r="C29" s="77"/>
-      <c r="D29" s="78"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41"/>
       <c r="E29" s="29"/>
       <c r="F29" s="23"/>
       <c r="G29" s="8"/>
@@ -1776,11 +1807,11 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="25"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="78"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="29"/>
       <c r="F30" s="23"/>
       <c r="G30" s="8"/>
@@ -1791,8 +1822,8 @@
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="25"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="78"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="29"/>
       <c r="F31" s="23"/>
       <c r="G31" s="8"/>
@@ -1803,8 +1834,8 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="25"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="78"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="41"/>
       <c r="E32" s="29"/>
       <c r="F32" s="23"/>
       <c r="G32" s="8"/>
@@ -1815,8 +1846,8 @@
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="26"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="80"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="43"/>
       <c r="E33" s="30"/>
       <c r="F33" s="24"/>
       <c r="G33" s="10"/>
@@ -1825,18 +1856,21 @@
       <c r="J33" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
+  <mergeCells count="34">
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="I1:J2"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -1846,16 +1880,17 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C1:H2"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="I1:J2"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da Lista de Requisitos para sprint #1
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3DBE68-E79C-419B-80A1-DA6B3FA814D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4554B3A9-C45E-4D11-8CDB-E44B6278C73F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -407,7 +407,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -858,127 +858,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1010,25 +902,133 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1049,7 +1049,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1347,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,32 +1365,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1398,60 +1398,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="78"/>
+      <c r="C5" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="46" t="s">
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="47"/>
-      <c r="I5" s="29" t="s">
+      <c r="H5" s="78"/>
+      <c r="I5" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="30"/>
+      <c r="J5" s="61"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="41" t="s">
+      <c r="B6" s="80"/>
+      <c r="C6" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="48" t="s">
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="49"/>
-      <c r="I6" s="31">
+      <c r="H6" s="80"/>
+      <c r="I6" s="62">
         <v>44046</v>
       </c>
-      <c r="J6" s="32"/>
+      <c r="J6" s="63"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="44" t="s">
+      <c r="B7" s="76"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="34"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="65"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1498,11 +1498,11 @@
       <c r="C12" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="80" t="s">
+      <c r="D12" s="55"/>
+      <c r="E12" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="79" t="s">
+      <c r="F12" s="40" t="s">
         <v>61</v>
       </c>
       <c r="G12" s="10" t="s">
@@ -1514,7 +1514,7 @@
       <c r="I12" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="23" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1525,14 +1525,14 @@
       <c r="B13" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="77"/>
-      <c r="E13" s="81" t="s">
+      <c r="D13" s="45"/>
+      <c r="E13" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G13" s="13" t="s">
@@ -1544,7 +1544,7 @@
       <c r="I13" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="60" t="s">
+      <c r="J13" s="24" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1555,14 +1555,14 @@
       <c r="B14" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="77"/>
-      <c r="E14" s="81" t="s">
+      <c r="D14" s="45"/>
+      <c r="E14" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="55" t="s">
+      <c r="F14" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G14" s="13" t="s">
@@ -1574,7 +1574,7 @@
       <c r="I14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="60" t="s">
+      <c r="J14" s="24" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1585,14 +1585,14 @@
       <c r="B15" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="81" t="s">
+      <c r="D15" s="45"/>
+      <c r="E15" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="55" t="s">
+      <c r="F15" s="20" t="s">
         <v>61</v>
       </c>
       <c r="G15" s="13" t="s">
@@ -1604,7 +1604,7 @@
       <c r="I15" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="24" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1615,14 +1615,14 @@
       <c r="B16" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="81" t="s">
+      <c r="D16" s="45"/>
+      <c r="E16" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="20" t="s">
         <v>67</v>
       </c>
       <c r="G16" s="13" t="s">
@@ -1634,7 +1634,7 @@
       <c r="I16" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="60" t="s">
+      <c r="J16" s="24" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1642,17 +1642,17 @@
       <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="77"/>
-      <c r="E17" s="81" t="s">
+      <c r="D17" s="45"/>
+      <c r="E17" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G17" s="13" t="s">
@@ -1664,7 +1664,7 @@
       <c r="I17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="60">
+      <c r="J17" s="24">
         <v>43906</v>
       </c>
     </row>
@@ -1675,14 +1675,14 @@
       <c r="B18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="77"/>
-      <c r="E18" s="82" t="s">
+      <c r="D18" s="45"/>
+      <c r="E18" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="20" t="s">
         <v>73</v>
       </c>
       <c r="G18" s="13" t="s">
@@ -1694,7 +1694,7 @@
       <c r="I18" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="60" t="s">
+      <c r="J18" s="24" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1702,17 +1702,17 @@
       <c r="A19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="77"/>
-      <c r="E19" s="82" t="s">
+      <c r="D19" s="45"/>
+      <c r="E19" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="20" t="s">
         <v>76</v>
       </c>
       <c r="G19" s="13" t="s">
@@ -1724,7 +1724,7 @@
       <c r="I19" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="60">
+      <c r="J19" s="24">
         <v>43880</v>
       </c>
     </row>
@@ -1735,14 +1735,14 @@
       <c r="B20" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="77"/>
-      <c r="E20" s="82" t="s">
+      <c r="D20" s="45"/>
+      <c r="E20" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="55" t="s">
+      <c r="F20" s="20" t="s">
         <v>76</v>
       </c>
       <c r="G20" s="13" t="s">
@@ -1754,7 +1754,7 @@
       <c r="I20" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="60" t="s">
+      <c r="J20" s="24" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1765,14 +1765,14 @@
       <c r="B21" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="77"/>
-      <c r="E21" s="82" t="s">
+      <c r="D21" s="45"/>
+      <c r="E21" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="55" t="s">
+      <c r="F21" s="20" t="s">
         <v>76</v>
       </c>
       <c r="G21" s="13" t="s">
@@ -1784,7 +1784,7 @@
       <c r="I21" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="60" t="s">
+      <c r="J21" s="24" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1795,14 +1795,14 @@
       <c r="B22" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="77"/>
-      <c r="E22" s="81" t="s">
+      <c r="D22" s="45"/>
+      <c r="E22" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="55" t="s">
+      <c r="F22" s="20" t="s">
         <v>76</v>
       </c>
       <c r="G22" s="13" t="s">
@@ -1814,7 +1814,7 @@
       <c r="I22" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="60" t="s">
+      <c r="J22" s="24" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1825,14 +1825,14 @@
       <c r="B23" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="77"/>
-      <c r="E23" s="82" t="s">
+      <c r="D23" s="45"/>
+      <c r="E23" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="55" t="s">
+      <c r="F23" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G23" s="13" t="s">
@@ -1844,7 +1844,7 @@
       <c r="I23" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J23" s="60" t="s">
+      <c r="J23" s="24" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1852,17 +1852,17 @@
       <c r="A24" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="77"/>
-      <c r="E24" s="82" t="s">
+      <c r="D24" s="45"/>
+      <c r="E24" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="55" t="s">
+      <c r="F24" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G24" s="13" t="s">
@@ -1874,7 +1874,7 @@
       <c r="I24" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="60">
+      <c r="J24" s="24">
         <v>43902</v>
       </c>
     </row>
@@ -1882,17 +1882,17 @@
       <c r="A25" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D25" s="77"/>
-      <c r="E25" s="82" t="s">
+      <c r="D25" s="45"/>
+      <c r="E25" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="55" t="s">
+      <c r="F25" s="20" t="s">
         <v>64</v>
       </c>
       <c r="G25" s="13" t="s">
@@ -1904,7 +1904,7 @@
       <c r="I25" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="J25" s="60">
+      <c r="J25" s="24">
         <v>43908</v>
       </c>
     </row>
@@ -1912,477 +1912,475 @@
       <c r="A26" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="73" t="s">
+      <c r="B26" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="82" t="s">
+      <c r="C26" s="81"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="55"/>
+      <c r="F26" s="20"/>
       <c r="G26" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="61" t="s">
+      <c r="I26" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J26" s="60"/>
+      <c r="J26" s="24"/>
     </row>
     <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="73" t="s">
+      <c r="B27" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="82" t="s">
+      <c r="C27" s="81"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="55"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="14"/>
-      <c r="I27" s="61" t="s">
+      <c r="I27" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J27" s="60"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="73" t="s">
+      <c r="B28" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="82" t="s">
+      <c r="C28" s="81"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="55"/>
+      <c r="F28" s="20"/>
       <c r="G28" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H28" s="14"/>
-      <c r="I28" s="61" t="s">
+      <c r="I28" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J28" s="60"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="78"/>
-      <c r="E29" s="82" t="s">
+      <c r="C29" s="81"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="55"/>
+      <c r="F29" s="20"/>
       <c r="G29" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="14"/>
-      <c r="I29" s="61" t="s">
+      <c r="I29" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J29" s="60"/>
+      <c r="J29" s="24"/>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="73" t="s">
+      <c r="B30" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="82" t="s">
+      <c r="C30" s="81"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="55"/>
+      <c r="F30" s="20"/>
       <c r="G30" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H30" s="14"/>
-      <c r="I30" s="61" t="s">
+      <c r="I30" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J30" s="60"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="73" t="s">
+      <c r="B31" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="82" t="s">
+      <c r="C31" s="81"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="F31" s="55"/>
+      <c r="F31" s="20"/>
       <c r="G31" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="14"/>
-      <c r="I31" s="61" t="s">
+      <c r="I31" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J31" s="60"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="B32" s="73" t="s">
+      <c r="B32" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C32" s="56"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="82" t="s">
+      <c r="C32" s="81"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="55"/>
+      <c r="F32" s="20"/>
       <c r="G32" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="14"/>
-      <c r="I32" s="61" t="s">
+      <c r="I32" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J32" s="60"/>
+      <c r="J32" s="24"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="73" t="s">
+      <c r="B33" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="56"/>
-      <c r="D33" s="78"/>
-      <c r="E33" s="82" t="s">
+      <c r="C33" s="81"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="55"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H33" s="14"/>
-      <c r="I33" s="61" t="s">
+      <c r="I33" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J33" s="60"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B34" s="70" t="s">
+      <c r="B34" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="68"/>
-      <c r="D34" s="68"/>
-      <c r="E34" s="82" t="s">
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="68"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="68"/>
-      <c r="I34" s="61" t="s">
+      <c r="H34" s="32"/>
+      <c r="I34" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J34" s="69"/>
+      <c r="J34" s="33"/>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B35" s="70" t="s">
+      <c r="B35" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="68"/>
-      <c r="D35" s="68"/>
-      <c r="E35" s="82" t="s">
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="68"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="68"/>
-      <c r="I35" s="61" t="s">
+      <c r="H35" s="32"/>
+      <c r="I35" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J35" s="69"/>
+      <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="B36" s="70" t="s">
+      <c r="B36" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="82" t="s">
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="68"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="68"/>
-      <c r="I36" s="61" t="s">
+      <c r="H36" s="32"/>
+      <c r="I36" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J36" s="69"/>
+      <c r="J36" s="33"/>
     </row>
     <row r="37" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="80" t="s">
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="68"/>
+      <c r="F37" s="32"/>
       <c r="G37" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="68"/>
-      <c r="I37" s="61" t="s">
+      <c r="H37" s="32"/>
+      <c r="I37" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J37" s="69"/>
+      <c r="J37" s="33"/>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="B38" s="70" t="s">
+      <c r="B38" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="80" t="s">
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="F38" s="68"/>
+      <c r="F38" s="32"/>
       <c r="G38" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="68"/>
-      <c r="I38" s="61" t="s">
+      <c r="H38" s="32"/>
+      <c r="I38" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J38" s="69"/>
+      <c r="J38" s="33"/>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B39" s="70" t="s">
+      <c r="B39" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="C39" s="68"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="82" t="s">
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F39" s="68"/>
+      <c r="F39" s="32"/>
       <c r="G39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="68"/>
-      <c r="I39" s="61" t="s">
+      <c r="H39" s="32"/>
+      <c r="I39" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J39" s="69"/>
+      <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B40" s="70" t="s">
+      <c r="B40" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="82" t="s">
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="68"/>
+      <c r="F40" s="32"/>
       <c r="G40" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="68"/>
-      <c r="I40" s="61" t="s">
+      <c r="H40" s="32"/>
+      <c r="I40" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J40" s="69"/>
+      <c r="J40" s="33"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B41" s="70" t="s">
+      <c r="B41" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="82" t="s">
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="F41" s="68"/>
+      <c r="F41" s="32"/>
       <c r="G41" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H41" s="68"/>
-      <c r="I41" s="61" t="s">
+      <c r="H41" s="32"/>
+      <c r="I41" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="J41" s="69"/>
+      <c r="J41" s="33"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="62"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="62"/>
-      <c r="I42" s="66"/>
-      <c r="J42" s="63"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="27"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="71"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="62"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="26"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="62"/>
-      <c r="I43" s="66"/>
-      <c r="J43" s="63"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="71"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="62"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="26"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="62"/>
-      <c r="I44" s="66"/>
-      <c r="J44" s="63"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="30"/>
+      <c r="J44" s="27"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
-      <c r="B45" s="71"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="62"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="26"/>
       <c r="G45" s="7"/>
-      <c r="H45" s="62"/>
-      <c r="I45" s="66"/>
-      <c r="J45" s="63"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
-      <c r="B46" s="71"/>
-      <c r="C46" s="62"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="62"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="26"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="62"/>
-      <c r="I46" s="66"/>
-      <c r="J46" s="63"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="27"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="71"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="62"/>
-      <c r="E47" s="74"/>
-      <c r="F47" s="62"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="26"/>
       <c r="G47" s="7"/>
-      <c r="H47" s="62"/>
-      <c r="I47" s="66"/>
-      <c r="J47" s="63"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="27"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="71"/>
-      <c r="C48" s="62"/>
-      <c r="D48" s="62"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="62"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="26"/>
       <c r="G48" s="7"/>
-      <c r="H48" s="62"/>
-      <c r="I48" s="66"/>
-      <c r="J48" s="63"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="27"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="74"/>
-      <c r="F49" s="62"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="26"/>
       <c r="G49" s="7"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="66"/>
-      <c r="J49" s="63"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="27"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
-      <c r="B50" s="72"/>
-      <c r="C50" s="64"/>
-      <c r="D50" s="64"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="64"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="28"/>
       <c r="G50" s="8"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="65"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="31"/>
+      <c r="J50" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C1:H2"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="I5:J5"/>
@@ -2397,17 +2395,19 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C1:H2"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da classe GEEventHandler
Inclusão da função virtual keyboardSpecialEvent
Inclusão dos eventos de teclado em GEWinApiWrapper
Inclusão de novos casos de teste para eventos de mouse e teclado
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141ACA8D-1503-4680-9FEA-1AC8F90EAA2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687EECB1-1DFC-4877-9B49-1741EEB2AB8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="128">
   <si>
     <t>BPM Game Engine</t>
   </si>
@@ -93,316 +93,328 @@
     <t>#6</t>
   </si>
   <si>
+    <t>#10</t>
+  </si>
+  <si>
+    <t>#11</t>
+  </si>
+  <si>
+    <t>#14</t>
+  </si>
+  <si>
+    <t>#15</t>
+  </si>
+  <si>
+    <t>#16</t>
+  </si>
+  <si>
+    <t>#17</t>
+  </si>
+  <si>
+    <t>#19</t>
+  </si>
+  <si>
+    <t>#20</t>
+  </si>
+  <si>
+    <t>Sistema de Janelas</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Finalizada</t>
+  </si>
+  <si>
+    <t>Customizar uma janela de aplicação</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>27/02/2020</t>
+  </si>
+  <si>
+    <t>Core Engine</t>
+  </si>
+  <si>
+    <t>Personalizar uma janela de aplicação antes de sua criação. Tipos possíveis de personalização: posicionamento inicial da janela, diferentes tipos de tamanho, diferente estilos*, texto do título da janela, tela cheia ou popup. (*) Consulte o documento "Guia de Desenvolvimento" para obter mais detalhes sobres todos os estilos possíveis de janela que podem ser criados.</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto Game Engine</t>
+  </si>
+  <si>
+    <t>Sistema de Entrada e Saída</t>
+  </si>
+  <si>
+    <t>21/02/2020</t>
+  </si>
+  <si>
+    <t>23/02/2020</t>
+  </si>
+  <si>
+    <t>Definir diferentes modos de renderização</t>
+  </si>
+  <si>
+    <t>Configurar diferentes modos de renderização como o formato do pixel, double buffering, buffer de pronfudidade.</t>
+  </si>
+  <si>
+    <t>Sistema de Renderização</t>
+  </si>
+  <si>
+    <t>24/02/2020</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>NOME</t>
+  </si>
+  <si>
+    <t>COMPONENTE</t>
+  </si>
+  <si>
+    <t>DEPENDÊNCIA</t>
+  </si>
+  <si>
+    <t>SPRINT</t>
+  </si>
+  <si>
+    <t>PRIORIDADE</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GEWindow e configurar todos os seus atributos.</t>
+  </si>
+  <si>
+    <t>Criar uma janela de aplicação no Microsoft Windows com um objeto GEWindow.</t>
+  </si>
+  <si>
+    <t>ApiWrapper</t>
+  </si>
+  <si>
+    <t>Destruir uma janela de aplicação no Microsoft Windows utilizando a classe Window.</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GameEngine passando uma referência a um objeto da classe ApiWrapper no construtor.</t>
+  </si>
+  <si>
+    <t>ApiWrapper WinApiWrapper</t>
+  </si>
+  <si>
+    <t>GEEventHandler</t>
+  </si>
+  <si>
+    <t>Iniciar o loop principal da Game Engine</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GameEngine passando uma referência a um objeto da classe ApiWrapper no construtor e executar o loop principal do motor de jogo.</t>
+  </si>
+  <si>
+    <t>Chamar métodos de uma classe herdada de ApiWrapper (polimorfismo)</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe WinApiWrapper, atribui-lo a um ponteiro para ApiWrapper. Então, chamar os métodos definidos em WinApiWrapper através do ponteiro para ApiWrapper.</t>
+  </si>
+  <si>
+    <t>Camada Multiplataforma</t>
+  </si>
+  <si>
+    <t>WinApiWrapper</t>
+  </si>
+  <si>
+    <t>ApiWrapper WinApiWrapper GEEventHandler</t>
+  </si>
+  <si>
+    <t>#9</t>
+  </si>
+  <si>
+    <t>Capturar diversas informações relacionadas ao movimento do mouse e o pressionamento de botões do mouse.</t>
+  </si>
+  <si>
+    <t>Capturar os eventos de entrada de teclado</t>
+  </si>
+  <si>
+    <t>Capturar os eventos de entrada de mouse</t>
+  </si>
+  <si>
+    <t>Capturar diversas informações relacionadas ao pressionamento de teclas do teclado, incluindo caracteres ASCII, caracteres especiais (por exemplo, CTRL, SHIFT, F1 e HOME) e pressionamento múltiplo de telcas.</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>Obter o tempo de execução de um quadro</t>
+  </si>
+  <si>
+    <t>Obter o tempo de execução de um quadro através da classe TimeHandler.</t>
+  </si>
+  <si>
+    <t>Gerenciador de Tempo</t>
+  </si>
+  <si>
+    <t>Calcular a quantidade de quadros por segundo</t>
+  </si>
+  <si>
+    <t>Obter o número de quadros executados por segundo.</t>
+  </si>
+  <si>
+    <t>Sistema de Entidades</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Definir o tipo de contexto do motor de jogo (2D ou 3D)</t>
+  </si>
+  <si>
+    <t>Sistema de Física</t>
+  </si>
+  <si>
+    <t>Criar o mundo no contexto 2D (matriz quadrada)</t>
+  </si>
+  <si>
+    <t>Sistema de Níveis</t>
+  </si>
+  <si>
+    <t>Aplicar uma textura em objetos Sprite</t>
+  </si>
+  <si>
+    <t>Gerenciamento de Assets</t>
+  </si>
+  <si>
+    <t>#21</t>
+  </si>
+  <si>
+    <t>Ler arquivos BPMN</t>
+  </si>
+  <si>
+    <t>#22</t>
+  </si>
+  <si>
+    <t>BPMN Parser</t>
+  </si>
+  <si>
+    <t>Exibir o log de execução do motor de jogo</t>
+  </si>
+  <si>
+    <t>Sistema de Log</t>
+  </si>
+  <si>
+    <t>Criar um objeto Sprite (contexto 2D)</t>
+  </si>
+  <si>
+    <t>Configurar os tipos de relacionamentos possíveis entres os Sprites (contexto 2D)</t>
+  </si>
+  <si>
+    <t>#23</t>
+  </si>
+  <si>
+    <t>Exibir informações do sistema</t>
+  </si>
+  <si>
+    <t>Controle de janelas ativa ou desativa (background)</t>
+  </si>
+  <si>
+    <t>reconfigirar viewport (sistema de renderização)</t>
+  </si>
+  <si>
+    <t>Método para redimensionar a janela programaticamente</t>
+  </si>
+  <si>
+    <t>Método para reposicionar a janela programaticamente</t>
+  </si>
+  <si>
+    <t>#24</t>
+  </si>
+  <si>
+    <t>#25</t>
+  </si>
+  <si>
+    <t>#26</t>
+  </si>
+  <si>
+    <t>#27</t>
+  </si>
+  <si>
+    <t>#28</t>
+  </si>
+  <si>
+    <t>#29</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto Timer</t>
+  </si>
+  <si>
+    <t>Inclusão de Frame Rate Governing</t>
+  </si>
+  <si>
+    <t>Implementação da classe Timer</t>
+  </si>
+  <si>
+    <t>#30</t>
+  </si>
+  <si>
+    <t>#31</t>
+  </si>
+  <si>
+    <t>Instanciar uma janela de aplicação</t>
+  </si>
+  <si>
+    <t>Criar uma janela de aplicação (Windows)</t>
+  </si>
+  <si>
+    <t>Destruir uma janela de aplicação (Windows)</t>
+  </si>
+  <si>
+    <t>Exibir uma janela de aplicação na tela</t>
+  </si>
+  <si>
+    <t>Exibir a janela de aplicação criada anteriormente no Microsoft Windows.</t>
+  </si>
+  <si>
+    <t>Configurar um estilo de janela de aplicação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configurar um estilo de janela de aplicação (GE_WIN_SPLASH, GE_WIN_DEFAULT, GE_WIN_DEFAULT_NO_SYS, GE_WIN_WINDOWED_FULLSCREEN, GE_WIN_COMPLETE). </t>
+  </si>
+  <si>
+    <t>Médio</t>
+  </si>
+  <si>
     <t>#7</t>
   </si>
   <si>
+    <t>Definir uma classe de eventos de usuário</t>
+  </si>
+  <si>
+    <t>Criar uma nova classe que herde da classe GEEventHandler e definir as funções de eventos do usuário.</t>
+  </si>
+  <si>
     <t>#8</t>
   </si>
   <si>
-    <t>#10</t>
-  </si>
-  <si>
-    <t>#11</t>
-  </si>
-  <si>
-    <t>#14</t>
-  </si>
-  <si>
-    <t>#15</t>
-  </si>
-  <si>
-    <t>#16</t>
-  </si>
-  <si>
-    <t>#17</t>
-  </si>
-  <si>
-    <t>#19</t>
-  </si>
-  <si>
-    <t>#20</t>
-  </si>
-  <si>
-    <t>Sistema de Janelas</t>
-  </si>
-  <si>
-    <t>Alta</t>
-  </si>
-  <si>
-    <t>Finalizada</t>
-  </si>
-  <si>
-    <t>18/02/2020</t>
-  </si>
-  <si>
-    <t>Customizar uma janela de aplicação</t>
-  </si>
-  <si>
-    <t>Baixa</t>
-  </si>
-  <si>
-    <t>27/02/2020</t>
-  </si>
-  <si>
-    <t>Core Engine</t>
-  </si>
-  <si>
-    <t>20/02/2020</t>
-  </si>
-  <si>
-    <t>Personalizar uma janela de aplicação antes de sua criação. Tipos possíveis de personalização: posicionamento inicial da janela, diferentes tipos de tamanho, diferente estilos*, texto do título da janela, tela cheia ou popup. (*) Consulte o documento "Guia de Desenvolvimento" para obter mais detalhes sobres todos os estilos possíveis de janela que podem ser criados.</t>
-  </si>
-  <si>
-    <t>25/02/2020</t>
-  </si>
-  <si>
-    <t>Instanciar um objeto Game Engine</t>
-  </si>
-  <si>
-    <t>Sistema de Entrada e Saída</t>
-  </si>
-  <si>
-    <t>21/02/2020</t>
-  </si>
-  <si>
-    <t>23/02/2020</t>
-  </si>
-  <si>
-    <t>Definir diferentes modos de renderização</t>
-  </si>
-  <si>
-    <t>Configurar diferentes modos de renderização como o formato do pixel, double buffering, buffer de pronfudidade.</t>
-  </si>
-  <si>
-    <t>Sistema de Renderização</t>
-  </si>
-  <si>
-    <t>24/02/2020</t>
-  </si>
-  <si>
-    <t>DESCRIÇÃO</t>
-  </si>
-  <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>COMPONENTE</t>
-  </si>
-  <si>
-    <t>DEPENDÊNCIA</t>
-  </si>
-  <si>
-    <t>SPRINT</t>
-  </si>
-  <si>
-    <t>PRIORIDADE</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>Instanciar um objeto da classe GEWindow e configurar todos os seus atributos.</t>
-  </si>
-  <si>
-    <t>Criar uma janela de aplicação no Microsoft Windows com um objeto GEWindow.</t>
-  </si>
-  <si>
-    <t>ApiWrapper</t>
-  </si>
-  <si>
-    <t>Destruir uma janela de aplicação no Microsoft Windows utilizando a classe Window.</t>
-  </si>
-  <si>
-    <t>Instanciar um objeto da classe GameEngine passando uma referência a um objeto da classe ApiWrapper no construtor.</t>
-  </si>
-  <si>
-    <t>ApiWrapper WinApiWrapper</t>
-  </si>
-  <si>
-    <t>Definir funções de eventos globais</t>
-  </si>
-  <si>
-    <t>Criar uma nova classe que herde da classe GEEventHandler e definir as funções de eventos globais do usuário.</t>
-  </si>
-  <si>
-    <t>GEEventHandler</t>
-  </si>
-  <si>
-    <t>Iniciar o loop principal da Game Engine</t>
-  </si>
-  <si>
-    <t>Instanciar um objeto da classe GameEngine passando uma referência a um objeto da classe ApiWrapper no construtor e executar o loop principal do motor de jogo.</t>
-  </si>
-  <si>
-    <t>Chamar métodos de uma classe herdada de ApiWrapper (polimorfismo)</t>
-  </si>
-  <si>
-    <t>Instanciar um objeto da classe WinApiWrapper, atribui-lo a um ponteiro para ApiWrapper. Então, chamar os métodos definidos em WinApiWrapper através do ponteiro para ApiWrapper.</t>
-  </si>
-  <si>
-    <t>Camada Multiplataforma</t>
-  </si>
-  <si>
-    <t>WinApiWrapper</t>
-  </si>
-  <si>
-    <t>Exibir uma janela de aplicação</t>
-  </si>
-  <si>
-    <t>Exibir a janela de aplicação.</t>
-  </si>
-  <si>
-    <t>ApiWrapper WinApiWrapper GEEventHandler</t>
-  </si>
-  <si>
-    <t>#9</t>
-  </si>
-  <si>
-    <t>Capturar diversas informações relacionadas ao movimento do mouse e o pressionamento de botões do mouse.</t>
-  </si>
-  <si>
-    <t>Capturar os eventos de entrada de teclado</t>
-  </si>
-  <si>
-    <t>Capturar os eventos de entrada de mouse</t>
-  </si>
-  <si>
-    <t>Capturar diversas informações relacionadas ao pressionamento de teclas do teclado, incluindo caracteres ASCII, caracteres especiais (por exemplo, CTRL, SHIFT, F1 e HOME) e pressionamento múltiplo de telcas.</t>
-  </si>
-  <si>
-    <t>#12</t>
-  </si>
-  <si>
-    <t>#13</t>
-  </si>
-  <si>
-    <t>Obter o tempo de execução de um quadro</t>
-  </si>
-  <si>
-    <t>Obter o tempo de execução de um quadro através da classe TimeHandler.</t>
-  </si>
-  <si>
-    <t>Gerenciador de Tempo</t>
-  </si>
-  <si>
-    <t>Calcular a quantidade de quadros por segundo</t>
-  </si>
-  <si>
-    <t>Obter o número de quadros executados por segundo.</t>
-  </si>
-  <si>
-    <t>Sistema de Entidades</t>
-  </si>
-  <si>
-    <t>Pendente</t>
-  </si>
-  <si>
-    <t>Definir o tipo de contexto do motor de jogo (2D ou 3D)</t>
-  </si>
-  <si>
-    <t>Sistema de Física</t>
-  </si>
-  <si>
-    <t>Criar o mundo no contexto 2D (matriz quadrada)</t>
-  </si>
-  <si>
-    <t>Sistema de Níveis</t>
-  </si>
-  <si>
-    <t>Aplicar uma textura em objetos Sprite</t>
-  </si>
-  <si>
-    <t>Gerenciamento de Assets</t>
-  </si>
-  <si>
-    <t>#21</t>
-  </si>
-  <si>
-    <t>Ler arquivos BPMN</t>
-  </si>
-  <si>
-    <t>#22</t>
-  </si>
-  <si>
-    <t>BPMN Parser</t>
-  </si>
-  <si>
-    <t>Exibir o log de execução do motor de jogo</t>
-  </si>
-  <si>
-    <t>Sistema de Log</t>
-  </si>
-  <si>
-    <t>Criar um objeto Sprite (contexto 2D)</t>
-  </si>
-  <si>
-    <t>Configurar os tipos de relacionamentos possíveis entres os Sprites (contexto 2D)</t>
-  </si>
-  <si>
-    <t>#23</t>
-  </si>
-  <si>
-    <t>Exibir informações do sistema</t>
-  </si>
-  <si>
-    <t>Controle de janelas ativa ou desativa (background)</t>
-  </si>
-  <si>
-    <t>reconfigirar viewport (sistema de renderização)</t>
-  </si>
-  <si>
-    <t>inicialização do sistema de renderização</t>
-  </si>
-  <si>
-    <t>Método para redimensionar a janela programaticamente</t>
-  </si>
-  <si>
-    <t>Método para reposicionar a janela programaticamente</t>
-  </si>
-  <si>
-    <t>#24</t>
-  </si>
-  <si>
-    <t>#25</t>
-  </si>
-  <si>
-    <t>#26</t>
-  </si>
-  <si>
-    <t>#27</t>
-  </si>
-  <si>
-    <t>#28</t>
-  </si>
-  <si>
-    <t>#29</t>
-  </si>
-  <si>
-    <t>Instanciar um objeto Timer</t>
-  </si>
-  <si>
-    <t>Inclusão de Frame Rate Governing</t>
-  </si>
-  <si>
-    <t>Implementação da classe Timer</t>
-  </si>
-  <si>
-    <t>#30</t>
-  </si>
-  <si>
-    <t>#31</t>
-  </si>
-  <si>
-    <t>Instanciar uma janela de aplicação</t>
-  </si>
-  <si>
-    <t>Criar uma janela de aplicação (Windows)</t>
-  </si>
-  <si>
-    <t>Destruir uma janela de aplicação (Windows)</t>
+    <t>Obter dados de entrada do mouse</t>
+  </si>
+  <si>
+    <t>Obter dados de entrada do teclado</t>
+  </si>
+  <si>
+    <t>Obter informações de entrada do mouse como posição do cursor na tela em pixels (eixo x e y) e o pressionamento dos botões esquerdo, meio e direito do mouse.</t>
+  </si>
+  <si>
+    <t>Obter informações de entrada do teclado como o pressionamento (e liberação) de todas as teclas do teclado.</t>
+  </si>
+  <si>
+    <t>Inicializar o sistema de renderização</t>
   </si>
 </sst>
 </file>
@@ -410,7 +422,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="[$-416]d/mmm/yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -802,7 +814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -870,23 +882,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -917,6 +920,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1032,6 +1044,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,29 +1487,29 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C11" s="79" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D11" s="80"/>
       <c r="E11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1496,29 +1517,29 @@
         <v>14</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C12" s="81" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D12" s="82"/>
-      <c r="E12" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>59</v>
+      <c r="E12" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>54</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="J12" s="39">
+        <v>43879</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1526,29 +1547,29 @@
         <v>15</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D13" s="47"/>
-      <c r="E13" s="42" t="s">
-        <v>30</v>
+      <c r="E13" s="37" t="s">
+        <v>28</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="J13" s="40">
+        <v>43877</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1556,74 +1577,74 @@
         <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D14" s="47"/>
-      <c r="E14" s="42" t="s">
-        <v>30</v>
+      <c r="E14" s="37" t="s">
+        <v>28</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J14" s="40">
+        <v>43879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="47"/>
-      <c r="E15" s="42" t="s">
-        <v>37</v>
+      <c r="E15" s="38" t="s">
+        <v>63</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J15" s="40">
+        <v>43881</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>63</v>
+      <c r="B16" s="21" t="s">
+        <v>114</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="D16" s="47"/>
-      <c r="E16" s="42" t="s">
-        <v>37</v>
+      <c r="E16" s="38" t="s">
+        <v>28</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>65</v>
@@ -1632,759 +1653,875 @@
         <v>14</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J16" s="40">
+        <v>43880</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>66</v>
+      <c r="B17" s="18" t="s">
+        <v>116</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>67</v>
+        <v>117</v>
       </c>
       <c r="D17" s="47"/>
-      <c r="E17" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>62</v>
-      </c>
+      <c r="E17" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="20"/>
       <c r="G17" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>31</v>
+        <v>118</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="24">
-        <v>43906</v>
+        <v>30</v>
+      </c>
+      <c r="J17" s="40">
+        <v>43880</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>68</v>
+        <v>119</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="D18" s="47"/>
-      <c r="E18" s="43" t="s">
-        <v>70</v>
+      <c r="E18" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J18" s="40">
+        <v>43886</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>72</v>
+        <v>122</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="D19" s="47"/>
-      <c r="E19" s="43" t="s">
-        <v>30</v>
+      <c r="E19" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J19" s="24">
-        <v>43880</v>
+        <v>30</v>
+      </c>
+      <c r="J19" s="40">
+        <v>43882</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>124</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="D20" s="47"/>
-      <c r="E20" s="43" t="s">
-        <v>42</v>
+      <c r="E20" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="J20" s="40">
+        <v>43884</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="85" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="83"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J21" s="24" t="s">
-        <v>44</v>
-      </c>
+      <c r="J21" s="41"/>
     </row>
     <row r="22" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="18" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="41"/>
+    </row>
+    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="43" t="s">
-        <v>47</v>
-      </c>
       <c r="F23" s="20" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G23" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>48</v>
+        <v>30</v>
+      </c>
+      <c r="J23" s="40">
+        <v>43881</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="D24" s="47"/>
-      <c r="E24" s="43" t="s">
-        <v>84</v>
+      <c r="E24" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>15</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="J24" s="24">
-        <v>43902</v>
+        <v>30</v>
+      </c>
+      <c r="J24" s="40">
+        <v>43906</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>85</v>
+        <v>66</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>69</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="D25" s="47"/>
-      <c r="E25" s="43" t="s">
-        <v>84</v>
+      <c r="E25" s="38" t="s">
+        <v>37</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="47"/>
+      <c r="E26" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="D27" s="47"/>
+      <c r="E27" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="J25" s="24">
-        <v>43908</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J26" s="24"/>
-    </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J27" s="24"/>
+      <c r="I27" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="40" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" s="20"/>
+      <c r="A28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="47"/>
+      <c r="E28" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="G28" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="14"/>
-      <c r="I28" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J28" s="24"/>
+        <v>14</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="40" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="20"/>
+        <v>72</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="G29" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="14"/>
-      <c r="I29" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J29" s="24"/>
+        <v>15</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="40">
+        <v>43902</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="43" t="s">
-        <v>94</v>
-      </c>
-      <c r="F30" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="47"/>
+      <c r="E30" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="20" t="s">
+        <v>57</v>
+      </c>
       <c r="G30" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="14"/>
-      <c r="I30" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J30" s="24"/>
+        <v>15</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="40">
+        <v>43908</v>
+      </c>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>96</v>
+        <v>23</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>80</v>
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="45"/>
-      <c r="E31" s="43" t="s">
-        <v>98</v>
+      <c r="E31" s="38" t="s">
+        <v>34</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="14"/>
-      <c r="I31" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J31" s="24"/>
+      <c r="I31" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" s="37" t="s">
-        <v>99</v>
+        <v>24</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>92</v>
       </c>
       <c r="C32" s="44"/>
       <c r="D32" s="45"/>
-      <c r="E32" s="43" t="s">
-        <v>100</v>
+      <c r="E32" s="38" t="s">
+        <v>78</v>
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="14"/>
-      <c r="I32" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J32" s="24"/>
+      <c r="I32" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J32" s="40"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>104</v>
+        <v>25</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>93</v>
       </c>
       <c r="C33" s="44"/>
       <c r="D33" s="45"/>
-      <c r="E33" s="43" t="s">
-        <v>37</v>
+      <c r="E33" s="38" t="s">
+        <v>81</v>
       </c>
       <c r="F33" s="20"/>
       <c r="G33" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H33" s="14"/>
-      <c r="I33" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J33" s="24"/>
+      <c r="I33" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="40"/>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B34" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="F34" s="32"/>
-      <c r="G34" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="32"/>
-      <c r="I34" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J34" s="33"/>
+        <v>26</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="44"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="20"/>
+      <c r="G34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="14"/>
+      <c r="I34" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" s="40"/>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B35" s="34" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="32"/>
-      <c r="I35" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="44"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="14"/>
+      <c r="I35" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J35" s="40"/>
+    </row>
+    <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="44"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="14"/>
+      <c r="I36" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J36" s="40"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="J35" s="33"/>
-    </row>
-    <row r="36" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="B36" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" s="32"/>
-      <c r="G36" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="32"/>
-      <c r="I36" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J36" s="33"/>
-    </row>
-    <row r="37" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B37" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F37" s="32"/>
-      <c r="G37" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J37" s="33"/>
-    </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="44"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="14"/>
+      <c r="I37" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J37" s="40"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" s="32"/>
-      <c r="I38" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J38" s="33"/>
+        <v>94</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" s="20"/>
+      <c r="G38" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="14"/>
+      <c r="I38" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="B39" s="34" t="s">
-        <v>116</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="32"/>
+        <v>100</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F39" s="28"/>
       <c r="G39" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J39" s="33"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J39" s="41"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="B40" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" s="32"/>
+        <v>101</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="28"/>
       <c r="G40" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="32"/>
-      <c r="I40" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J40" s="33"/>
-    </row>
-    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F41" s="32"/>
-      <c r="G41" s="14" t="s">
+      <c r="H40" s="28"/>
+      <c r="I40" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J40" s="41"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="23"/>
+      <c r="J41" s="41"/>
+    </row>
+    <row r="42" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F42" s="28"/>
+      <c r="G42" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H41" s="32"/>
-      <c r="I41" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="J41" s="33"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="27"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="30"/>
-      <c r="J43" s="27"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="27"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="30"/>
-      <c r="J45" s="27"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="27"/>
+      <c r="H42" s="28"/>
+      <c r="I42" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J42" s="41"/>
+    </row>
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" s="28"/>
+      <c r="G43" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H43" s="28"/>
+      <c r="I43" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J43" s="41"/>
+    </row>
+    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" s="28"/>
+      <c r="G44" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H44" s="28"/>
+      <c r="I44" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J44" s="41"/>
+    </row>
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="28"/>
+      <c r="G45" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H45" s="28"/>
+      <c r="I45" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J45" s="41"/>
+    </row>
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F46" s="28"/>
+      <c r="G46" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H46" s="28"/>
+      <c r="I46" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J46" s="41"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="26"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="24"/>
       <c r="G47" s="7"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="27"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="42"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="26"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="24"/>
       <c r="G48" s="7"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="27"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="42"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="35"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="26"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="24"/>
       <c r="G49" s="7"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="27"/>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="29"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="42"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="42"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="30"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="42"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="42"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="42"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="42"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="25"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="42">
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="I5:J5"/>
@@ -2400,17 +2537,17 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C1:H2"/>
+    <mergeCell ref="C33:D33"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Inclusão da classe GERenderingSystem
Implementação do método initializeRenderingSystem - GEApiWrapper
Inclusão do método swapBuffers - GEApiWrapper
Inclusão da referência a GERenderingSystem para GEWindow
Atualização de makefile para link da API OpenGL, GLU e GDI
Implementação do novo teste de unidade para GERenderingSystem
Callback de WM_SIZE em window procedure
Atualização de liberação de recursos de uma janela
Correção em outros testes de unidade apos a inclusão do novo feature
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687EECB1-1DFC-4877-9B49-1741EEB2AB8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD69CD9-B3B4-401B-A5D3-E2F4E0BB387D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="129">
   <si>
     <t>BPM Game Engine</t>
   </si>
@@ -339,9 +339,6 @@
     <t>#25</t>
   </si>
   <si>
-    <t>#26</t>
-  </si>
-  <si>
     <t>#27</t>
   </si>
   <si>
@@ -415,6 +412,12 @@
   </si>
   <si>
     <t>Inicializar o sistema de renderização</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicializar o sistema de renderização (OpenGL) a partir de uma referência para GERenderingSystem. Isto signigica configurar a viewport de OpenGL e a cor de fundo da janela. </t>
+  </si>
+  <si>
+    <t>ApiWrapper WinApiWrapper GEEventHandler GEWindow</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +507,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -814,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -929,132 +938,152 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,32 +1418,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="48" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="53"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="56"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="58"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1422,60 +1451,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="65" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="73" t="s">
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="56" t="s">
+      <c r="H5" s="77"/>
+      <c r="I5" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="57"/>
+      <c r="J5" s="60"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="68" t="s">
+      <c r="B6" s="79"/>
+      <c r="C6" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="75" t="s">
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="76"/>
-      <c r="I6" s="58">
+      <c r="H6" s="79"/>
+      <c r="I6" s="61">
         <v>44046</v>
       </c>
-      <c r="J6" s="59"/>
+      <c r="J6" s="62"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="71" t="s">
+      <c r="B7" s="75"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="72"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="61"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="64"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1489,10 +1518,10 @@
       <c r="B11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="80"/>
+      <c r="D11" s="48"/>
       <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1517,12 +1546,12 @@
         <v>14</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="81" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="82"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="36" t="s">
         <v>28</v>
       </c>
@@ -1547,12 +1576,12 @@
         <v>15</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="47"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="37" t="s">
         <v>28</v>
       </c>
@@ -1577,12 +1606,12 @@
         <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="47"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="37" t="s">
         <v>28</v>
       </c>
@@ -1609,10 +1638,10 @@
       <c r="B15" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="47"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="38" t="s">
         <v>63</v>
       </c>
@@ -1637,12 +1666,12 @@
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="C16" s="46" t="s">
-        <v>115</v>
-      </c>
-      <c r="D16" s="47"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
@@ -1667,12 +1696,12 @@
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="47"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="37" t="s">
         <v>28</v>
       </c>
@@ -1681,7 +1710,7 @@
         <v>14</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I17" s="16" t="s">
         <v>30</v>
@@ -1692,15 +1721,15 @@
     </row>
     <row r="18" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="37" t="s">
         <v>34</v>
       </c>
@@ -1722,15 +1751,15 @@
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" s="47"/>
+      <c r="C19" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" s="46"/>
       <c r="E19" s="37" t="s">
         <v>34</v>
       </c>
@@ -1741,7 +1770,7 @@
         <v>14</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>30</v>
@@ -1750,17 +1779,17 @@
         <v>43882</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20" s="47"/>
+        <v>123</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="46"/>
       <c r="E20" s="37" t="s">
         <v>34</v>
       </c>
@@ -1771,7 +1800,7 @@
         <v>14</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>30</v>
@@ -1780,39 +1809,47 @@
         <v>43884</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="C21" s="83"/>
       <c r="D21" s="84"/>
       <c r="E21" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="20" t="s">
+        <v>128</v>
+      </c>
       <c r="G21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J21" s="41"/>
-    </row>
-    <row r="22" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="41"/>
+      <c r="H21" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="40">
+        <v>43885</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="85"/>
+      <c r="B22" s="86"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="89"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="93"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
@@ -1821,10 +1858,10 @@
       <c r="B23" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="47"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="37" t="s">
         <v>34</v>
       </c>
@@ -1851,10 +1888,10 @@
       <c r="B24" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="46" t="s">
+      <c r="C24" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="47"/>
+      <c r="D24" s="46"/>
       <c r="E24" s="37" t="s">
         <v>34</v>
       </c>
@@ -1881,10 +1918,10 @@
       <c r="B25" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="46" t="s">
+      <c r="C25" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="47"/>
+      <c r="D25" s="46"/>
       <c r="E25" s="38" t="s">
         <v>37</v>
       </c>
@@ -1911,10 +1948,10 @@
       <c r="B26" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="47"/>
+      <c r="D26" s="46"/>
       <c r="E26" s="38" t="s">
         <v>37</v>
       </c>
@@ -1941,10 +1978,10 @@
       <c r="B27" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="47"/>
+      <c r="D27" s="46"/>
       <c r="E27" s="37" t="s">
         <v>28</v>
       </c>
@@ -1971,10 +2008,10 @@
       <c r="B28" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="46" t="s">
+      <c r="C28" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="47"/>
+      <c r="D28" s="46"/>
       <c r="E28" s="38" t="s">
         <v>42</v>
       </c>
@@ -2001,10 +2038,10 @@
       <c r="B29" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="46" t="s">
+      <c r="C29" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="47"/>
+      <c r="D29" s="46"/>
       <c r="E29" s="38" t="s">
         <v>75</v>
       </c>
@@ -2031,10 +2068,10 @@
       <c r="B30" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="47"/>
+      <c r="D30" s="46"/>
       <c r="E30" s="38" t="s">
         <v>75</v>
       </c>
@@ -2061,8 +2098,8 @@
       <c r="B31" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="44"/>
-      <c r="D31" s="45"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="83"/>
       <c r="E31" s="38" t="s">
         <v>34</v>
       </c>
@@ -2083,8 +2120,8 @@
       <c r="B32" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="45"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="83"/>
       <c r="E32" s="38" t="s">
         <v>78</v>
       </c>
@@ -2105,8 +2142,8 @@
       <c r="B33" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="44"/>
-      <c r="D33" s="45"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="83"/>
       <c r="E33" s="38" t="s">
         <v>81</v>
       </c>
@@ -2127,8 +2164,8 @@
       <c r="B34" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="45"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="83"/>
       <c r="E34" s="38" t="s">
         <v>83</v>
       </c>
@@ -2149,8 +2186,8 @@
       <c r="B35" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="83"/>
       <c r="E35" s="38" t="s">
         <v>85</v>
       </c>
@@ -2171,8 +2208,8 @@
       <c r="B36" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="45"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="83"/>
       <c r="E36" s="38" t="s">
         <v>89</v>
       </c>
@@ -2193,8 +2230,8 @@
       <c r="B37" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="45"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="83"/>
       <c r="E37" s="38" t="s">
         <v>91</v>
       </c>
@@ -2215,8 +2252,8 @@
       <c r="B38" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="45"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="83"/>
       <c r="E38" s="38" t="s">
         <v>34</v>
       </c>
@@ -2288,7 +2325,7 @@
     </row>
     <row r="42" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>98</v>
@@ -2310,7 +2347,7 @@
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" s="29" t="s">
         <v>99</v>
@@ -2332,10 +2369,10 @@
     </row>
     <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="29" t="s">
         <v>105</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>106</v>
       </c>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
@@ -2354,10 +2391,10 @@
     </row>
     <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
@@ -2376,10 +2413,10 @@
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
@@ -2505,23 +2542,18 @@
       <c r="J55" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
+  <mergeCells count="43">
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="I5:J5"/>
@@ -2537,17 +2569,23 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C1:H2"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização de todos os documentos do projeto
Inclusão das constantes simbólicas para cores de background
Correção no teste de unidade (variáveis globais com mesmo nome
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD69CD9-B3B4-401B-A5D3-E2F4E0BB387D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773DD916-53FD-4E16-80BC-CDD9F80B28C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
+    <workbookView xWindow="2370" yWindow="285" windowWidth="21600" windowHeight="11385" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -941,137 +941,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1084,6 +958,132 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1400,7 +1400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -1418,32 +1418,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="51" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="56"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="66"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="58"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="68"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1451,60 +1451,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="68" t="s">
+      <c r="B5" s="87"/>
+      <c r="C5" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="76" t="s">
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="77"/>
-      <c r="I5" s="59" t="s">
+      <c r="H5" s="87"/>
+      <c r="I5" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="60"/>
+      <c r="J5" s="70"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="79"/>
-      <c r="C6" s="71" t="s">
+      <c r="B6" s="89"/>
+      <c r="C6" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="78" t="s">
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="79"/>
-      <c r="I6" s="61">
+      <c r="H6" s="89"/>
+      <c r="I6" s="71">
         <v>44046</v>
       </c>
-      <c r="J6" s="62"/>
+      <c r="J6" s="72"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="74" t="s">
+      <c r="B7" s="85"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="75"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="64"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="74"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1518,10 +1518,10 @@
       <c r="B11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="48"/>
+      <c r="D11" s="56"/>
       <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
@@ -1548,10 +1548,10 @@
       <c r="B12" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="50"/>
+      <c r="D12" s="58"/>
       <c r="E12" s="36" t="s">
         <v>28</v>
       </c>
@@ -1578,10 +1578,10 @@
       <c r="B13" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="46"/>
+      <c r="D13" s="53"/>
       <c r="E13" s="37" t="s">
         <v>28</v>
       </c>
@@ -1608,10 +1608,10 @@
       <c r="B14" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="46"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="37" t="s">
         <v>28</v>
       </c>
@@ -1638,10 +1638,10 @@
       <c r="B15" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="46"/>
+      <c r="D15" s="53"/>
       <c r="E15" s="38" t="s">
         <v>63</v>
       </c>
@@ -1668,10 +1668,10 @@
       <c r="B16" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="46"/>
+      <c r="D16" s="53"/>
       <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
@@ -1698,10 +1698,10 @@
       <c r="B17" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="46"/>
+      <c r="D17" s="53"/>
       <c r="E17" s="37" t="s">
         <v>28</v>
       </c>
@@ -1726,10 +1726,10 @@
       <c r="B18" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="46"/>
+      <c r="D18" s="53"/>
       <c r="E18" s="37" t="s">
         <v>34</v>
       </c>
@@ -1756,10 +1756,10 @@
       <c r="B19" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="D19" s="46"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="37" t="s">
         <v>34</v>
       </c>
@@ -1786,10 +1786,10 @@
       <c r="B20" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="46"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="37" t="s">
         <v>34</v>
       </c>
@@ -1816,10 +1816,10 @@
       <c r="B21" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="84"/>
+      <c r="D21" s="54"/>
       <c r="E21" s="38" t="s">
         <v>42</v>
       </c>
@@ -1840,16 +1840,16 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="85"/>
-      <c r="B22" s="86"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="88"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="90"/>
-      <c r="G22" s="91"/>
-      <c r="H22" s="90"/>
-      <c r="I22" s="92"/>
-      <c r="J22" s="93"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="51"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
@@ -1858,10 +1858,10 @@
       <c r="B23" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="46"/>
+      <c r="D23" s="53"/>
       <c r="E23" s="37" t="s">
         <v>34</v>
       </c>
@@ -1888,10 +1888,10 @@
       <c r="B24" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="46"/>
+      <c r="D24" s="53"/>
       <c r="E24" s="37" t="s">
         <v>34</v>
       </c>
@@ -1918,10 +1918,10 @@
       <c r="B25" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="46"/>
+      <c r="D25" s="53"/>
       <c r="E25" s="38" t="s">
         <v>37</v>
       </c>
@@ -1948,10 +1948,10 @@
       <c r="B26" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="46"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="38" t="s">
         <v>37</v>
       </c>
@@ -1978,10 +1978,10 @@
       <c r="B27" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="46"/>
+      <c r="D27" s="53"/>
       <c r="E27" s="37" t="s">
         <v>28</v>
       </c>
@@ -2008,10 +2008,10 @@
       <c r="B28" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="46"/>
+      <c r="D28" s="53"/>
       <c r="E28" s="38" t="s">
         <v>42</v>
       </c>
@@ -2038,10 +2038,10 @@
       <c r="B29" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="46"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="38" t="s">
         <v>75</v>
       </c>
@@ -2068,10 +2068,10 @@
       <c r="B30" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C30" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="46"/>
+      <c r="D30" s="53"/>
       <c r="E30" s="38" t="s">
         <v>75</v>
       </c>
@@ -2098,8 +2098,8 @@
       <c r="B31" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="82"/>
-      <c r="D31" s="83"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="93"/>
       <c r="E31" s="38" t="s">
         <v>34</v>
       </c>
@@ -2120,8 +2120,8 @@
       <c r="B32" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="82"/>
-      <c r="D32" s="83"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="93"/>
       <c r="E32" s="38" t="s">
         <v>78</v>
       </c>
@@ -2142,8 +2142,8 @@
       <c r="B33" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="82"/>
-      <c r="D33" s="83"/>
+      <c r="C33" s="92"/>
+      <c r="D33" s="93"/>
       <c r="E33" s="38" t="s">
         <v>81</v>
       </c>
@@ -2164,8 +2164,8 @@
       <c r="B34" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="82"/>
-      <c r="D34" s="83"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="93"/>
       <c r="E34" s="38" t="s">
         <v>83</v>
       </c>
@@ -2186,8 +2186,8 @@
       <c r="B35" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="82"/>
-      <c r="D35" s="83"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="93"/>
       <c r="E35" s="38" t="s">
         <v>85</v>
       </c>
@@ -2208,8 +2208,8 @@
       <c r="B36" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="82"/>
-      <c r="D36" s="83"/>
+      <c r="C36" s="92"/>
+      <c r="D36" s="93"/>
       <c r="E36" s="38" t="s">
         <v>89</v>
       </c>
@@ -2230,8 +2230,8 @@
       <c r="B37" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C37" s="82"/>
-      <c r="D37" s="83"/>
+      <c r="C37" s="92"/>
+      <c r="D37" s="93"/>
       <c r="E37" s="38" t="s">
         <v>91</v>
       </c>
@@ -2252,8 +2252,8 @@
       <c r="B38" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="82"/>
-      <c r="D38" s="83"/>
+      <c r="C38" s="92"/>
+      <c r="D38" s="93"/>
       <c r="E38" s="38" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Atualização da classe GameEngine
Inicializando as variáveis para cálculo de frame time
Refatoração do código de avaliação
Atualização dos testes de unidade para Game Engine
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773DD916-53FD-4E16-80BC-CDD9F80B28C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B16F260-442F-4791-A5D5-62EF2C4DC211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="285" windowWidth="21600" windowHeight="11385" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="121">
   <si>
     <t>BPM Game Engine</t>
   </si>
@@ -126,33 +126,12 @@
     <t>Finalizada</t>
   </si>
   <si>
-    <t>Customizar uma janela de aplicação</t>
-  </si>
-  <si>
     <t>Baixa</t>
   </si>
   <si>
-    <t>27/02/2020</t>
-  </si>
-  <si>
     <t>Core Engine</t>
   </si>
   <si>
-    <t>Personalizar uma janela de aplicação antes de sua criação. Tipos possíveis de personalização: posicionamento inicial da janela, diferentes tipos de tamanho, diferente estilos*, texto do título da janela, tela cheia ou popup. (*) Consulte o documento "Guia de Desenvolvimento" para obter mais detalhes sobres todos os estilos possíveis de janela que podem ser criados.</t>
-  </si>
-  <si>
-    <t>Instanciar um objeto Game Engine</t>
-  </si>
-  <si>
-    <t>Sistema de Entrada e Saída</t>
-  </si>
-  <si>
-    <t>21/02/2020</t>
-  </si>
-  <si>
-    <t>23/02/2020</t>
-  </si>
-  <si>
     <t>Definir diferentes modos de renderização</t>
   </si>
   <si>
@@ -201,9 +180,6 @@
     <t>Destruir uma janela de aplicação no Microsoft Windows utilizando a classe Window.</t>
   </si>
   <si>
-    <t>Instanciar um objeto da classe GameEngine passando uma referência a um objeto da classe ApiWrapper no construtor.</t>
-  </si>
-  <si>
     <t>ApiWrapper WinApiWrapper</t>
   </si>
   <si>
@@ -213,9 +189,6 @@
     <t>Iniciar o loop principal da Game Engine</t>
   </si>
   <si>
-    <t>Instanciar um objeto da classe GameEngine passando uma referência a um objeto da classe ApiWrapper no construtor e executar o loop principal do motor de jogo.</t>
-  </si>
-  <si>
     <t>Chamar métodos de uma classe herdada de ApiWrapper (polimorfismo)</t>
   </si>
   <si>
@@ -234,30 +207,12 @@
     <t>#9</t>
   </si>
   <si>
-    <t>Capturar diversas informações relacionadas ao movimento do mouse e o pressionamento de botões do mouse.</t>
-  </si>
-  <si>
-    <t>Capturar os eventos de entrada de teclado</t>
-  </si>
-  <si>
-    <t>Capturar os eventos de entrada de mouse</t>
-  </si>
-  <si>
-    <t>Capturar diversas informações relacionadas ao pressionamento de teclas do teclado, incluindo caracteres ASCII, caracteres especiais (por exemplo, CTRL, SHIFT, F1 e HOME) e pressionamento múltiplo de telcas.</t>
-  </si>
-  <si>
     <t>#12</t>
   </si>
   <si>
     <t>#13</t>
   </si>
   <si>
-    <t>Obter o tempo de execução de um quadro</t>
-  </si>
-  <si>
-    <t>Obter o tempo de execução de um quadro através da classe TimeHandler.</t>
-  </si>
-  <si>
     <t>Gerenciador de Tempo</t>
   </si>
   <si>
@@ -418,6 +373,27 @@
   </si>
   <si>
     <t>ApiWrapper WinApiWrapper GEEventHandler GEWindow</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe Game Engine</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GameEngine.</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GameEngine, configurar os eventos de usuário e executar o loop principal do motor de jogo.</t>
+  </si>
+  <si>
+    <t>EventHandler</t>
+  </si>
+  <si>
+    <t>Obter o tempo de duração de um quadro da Game Engine</t>
+  </si>
+  <si>
+    <t>Obter o tempo de duração de um quadro da Game Engine através da classe TimeHandler.</t>
+  </si>
+  <si>
+    <t>TimeHandler GameEngine</t>
   </si>
 </sst>
 </file>
@@ -476,7 +452,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +489,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="26">
     <border>
@@ -823,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -959,130 +941,166 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1398,10 +1416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,32 +1436,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="61"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="63"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1451,60 +1469,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="86" t="s">
+      <c r="A5" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="78" t="s">
+      <c r="B5" s="82"/>
+      <c r="C5" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="86" t="s">
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="87"/>
-      <c r="I5" s="69" t="s">
+      <c r="H5" s="82"/>
+      <c r="I5" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="70"/>
+      <c r="J5" s="65"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="81" t="s">
+      <c r="B6" s="84"/>
+      <c r="C6" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="88" t="s">
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="89"/>
-      <c r="I6" s="71">
+      <c r="H6" s="84"/>
+      <c r="I6" s="66">
         <v>44046</v>
       </c>
-      <c r="J6" s="72"/>
+      <c r="J6" s="67"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="77"/>
-      <c r="G7" s="84" t="s">
+      <c r="B7" s="80"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="85"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="74"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1516,29 +1534,29 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="88"/>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1546,17 +1564,17 @@
         <v>14</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="58"/>
+        <v>95</v>
+      </c>
+      <c r="C12" s="89" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="90"/>
       <c r="E12" s="36" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>14</v>
@@ -1576,17 +1594,17 @@
         <v>15</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="53"/>
+        <v>96</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="55"/>
       <c r="E13" s="37" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>14</v>
@@ -1606,17 +1624,17 @@
         <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="53"/>
+        <v>97</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="55"/>
       <c r="E14" s="37" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>14</v>
@@ -1636,17 +1654,17 @@
         <v>17</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="53"/>
+        <v>52</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="55"/>
       <c r="E15" s="38" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>14</v>
@@ -1666,17 +1684,17 @@
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" s="53"/>
+        <v>98</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="55"/>
       <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>14</v>
@@ -1696,12 +1714,12 @@
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="53"/>
+        <v>100</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="55"/>
       <c r="E17" s="37" t="s">
         <v>28</v>
       </c>
@@ -1710,7 +1728,7 @@
         <v>14</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="I17" s="16" t="s">
         <v>30</v>
@@ -1721,26 +1739,26 @@
     </row>
     <row r="18" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="D18" s="53"/>
+        <v>104</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="55"/>
       <c r="E18" s="37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I18" s="16" t="s">
         <v>30</v>
@@ -1751,26 +1769,26 @@
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>124</v>
-      </c>
-      <c r="D19" s="53"/>
+        <v>107</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="55"/>
       <c r="E19" s="37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>30</v>
@@ -1781,26 +1799,26 @@
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="53"/>
+        <v>108</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="55"/>
       <c r="E20" s="37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F20" s="20" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>30</v>
@@ -1814,23 +1832,23 @@
         <v>20</v>
       </c>
       <c r="B21" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" s="52" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="54"/>
+        <v>111</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" s="93"/>
       <c r="E21" s="38" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="I21" s="16" t="s">
         <v>30</v>
@@ -1842,8 +1860,8 @@
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
       <c r="B22" s="46"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="60"/>
+      <c r="C22" s="91"/>
+      <c r="D22" s="92"/>
       <c r="E22" s="47"/>
       <c r="F22" s="48"/>
       <c r="G22" s="49"/>
@@ -1853,23 +1871,21 @@
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="53"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="94" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="55"/>
       <c r="E23" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>54</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F23" s="20"/>
       <c r="G23" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H23" s="14" t="s">
         <v>29</v>
@@ -1878,25 +1894,25 @@
         <v>30</v>
       </c>
       <c r="J23" s="40">
-        <v>43881</v>
+        <v>43890</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="52" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="53"/>
+        <v>58</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="55"/>
       <c r="E24" s="37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>57</v>
+        <v>117</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>15</v>
@@ -1908,266 +1924,182 @@
         <v>30</v>
       </c>
       <c r="J24" s="40">
-        <v>43906</v>
+        <v>43890</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="53"/>
+        <v>59</v>
+      </c>
+      <c r="B25" s="94" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="55"/>
       <c r="E25" s="38" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I25" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J25" s="40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="52" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="53"/>
-      <c r="E26" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" s="13" t="s">
+      <c r="J25" s="40">
+        <v>43891</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="40"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="40"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="40"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="40"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="97"/>
+      <c r="B30" s="95"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="100"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="102"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="104"/>
+      <c r="J30" s="105"/>
+    </row>
+    <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="55"/>
+      <c r="E31" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H26" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I26" s="16" t="s">
+      <c r="H31" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="52" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="53"/>
-      <c r="E27" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I27" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J27" s="40" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="53"/>
-      <c r="E28" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I28" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J28" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="53"/>
-      <c r="E29" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J29" s="40">
-        <v>43902</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C30" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="53"/>
-      <c r="E30" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" s="40">
-        <v>43908</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="92"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="14"/>
-      <c r="I31" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J31" s="40"/>
+      <c r="J31" s="40" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="C32" s="92"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="38" t="s">
-        <v>78</v>
-      </c>
+      <c r="A32" s="12"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="20"/>
-      <c r="G32" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="G32" s="13"/>
       <c r="H32" s="14"/>
-      <c r="I32" s="23" t="s">
-        <v>79</v>
-      </c>
+      <c r="I32" s="16"/>
       <c r="J32" s="40"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="92"/>
-      <c r="D33" s="93"/>
+        <v>22</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="55"/>
       <c r="E33" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" s="20"/>
+        <v>60</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>49</v>
+      </c>
       <c r="G33" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="14"/>
-      <c r="I33" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J33" s="40"/>
+        <v>15</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J33" s="40">
+        <v>43908</v>
+      </c>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="92"/>
-      <c r="D34" s="93"/>
+        <v>65</v>
+      </c>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
       <c r="E34" s="38" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="13" t="s">
@@ -2175,21 +2107,21 @@
       </c>
       <c r="H34" s="14"/>
       <c r="I34" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J34" s="40"/>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="92"/>
-      <c r="D35" s="93"/>
+        <v>77</v>
+      </c>
+      <c r="C35" s="52"/>
+      <c r="D35" s="53"/>
       <c r="E35" s="38" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="13" t="s">
@@ -2197,21 +2129,21 @@
       </c>
       <c r="H35" s="14"/>
       <c r="I35" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J35" s="40"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="92"/>
-      <c r="D36" s="93"/>
+        <v>78</v>
+      </c>
+      <c r="C36" s="52"/>
+      <c r="D36" s="53"/>
       <c r="E36" s="38" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="13" t="s">
@@ -2219,21 +2151,21 @@
       </c>
       <c r="H36" s="14"/>
       <c r="I36" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J36" s="40"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="92"/>
-      <c r="D37" s="93"/>
+        <v>67</v>
+      </c>
+      <c r="C37" s="52"/>
+      <c r="D37" s="53"/>
       <c r="E37" s="38" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="13" t="s">
@@ -2241,21 +2173,21 @@
       </c>
       <c r="H37" s="14"/>
       <c r="I37" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J37" s="40"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="92"/>
-      <c r="D38" s="93"/>
+        <v>69</v>
+      </c>
+      <c r="C38" s="52"/>
+      <c r="D38" s="53"/>
       <c r="E38" s="38" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="13" t="s">
@@ -2263,77 +2195,87 @@
       </c>
       <c r="H38" s="14"/>
       <c r="I38" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B39" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
+        <v>71</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="52"/>
+      <c r="D39" s="53"/>
       <c r="E39" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" s="28"/>
-      <c r="G39" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" s="28"/>
+        <v>74</v>
+      </c>
+      <c r="F39" s="20"/>
+      <c r="G39" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J39" s="41"/>
+        <v>64</v>
+      </c>
+      <c r="J39" s="40"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
+        <v>73</v>
+      </c>
+      <c r="B40" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="52"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="F40" s="28"/>
-      <c r="G40" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H40" s="28"/>
+        <v>76</v>
+      </c>
+      <c r="F40" s="20"/>
+      <c r="G40" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="14"/>
       <c r="I40" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J40" s="40"/>
+    </row>
+    <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="J40" s="41"/>
-    </row>
-    <row r="41" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="28"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="41"/>
-    </row>
-    <row r="42" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="52"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" s="20"/>
+      <c r="G41" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="14"/>
+      <c r="I41" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J41" s="40"/>
+    </row>
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C42" s="28"/>
       <c r="D42" s="28"/>
-      <c r="E42" s="36" t="s">
-        <v>28</v>
+      <c r="E42" s="38" t="s">
+        <v>32</v>
       </c>
       <c r="F42" s="28"/>
       <c r="G42" s="14" t="s">
@@ -2341,21 +2283,21 @@
       </c>
       <c r="H42" s="28"/>
       <c r="I42" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
-      <c r="E43" s="36" t="s">
-        <v>28</v>
+      <c r="E43" s="38" t="s">
+        <v>35</v>
       </c>
       <c r="F43" s="28"/>
       <c r="G43" s="14" t="s">
@@ -2363,43 +2305,33 @@
       </c>
       <c r="H43" s="28"/>
       <c r="I43" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J43" s="41"/>
     </row>
-    <row r="44" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>105</v>
-      </c>
+    <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="12"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="28"/>
       <c r="D44" s="28"/>
-      <c r="E44" s="38" t="s">
-        <v>75</v>
-      </c>
+      <c r="E44" s="38"/>
       <c r="F44" s="28"/>
-      <c r="G44" s="14" t="s">
-        <v>17</v>
-      </c>
+      <c r="G44" s="14"/>
       <c r="H44" s="28"/>
-      <c r="I44" s="23" t="s">
-        <v>79</v>
-      </c>
+      <c r="I44" s="23"/>
       <c r="J44" s="41"/>
     </row>
-    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
-      <c r="E45" s="38" t="s">
-        <v>75</v>
+      <c r="E45" s="36" t="s">
+        <v>28</v>
       </c>
       <c r="F45" s="28"/>
       <c r="G45" s="14" t="s">
@@ -2407,21 +2339,21 @@
       </c>
       <c r="H45" s="28"/>
       <c r="I45" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
-      <c r="E46" s="38" t="s">
-        <v>75</v>
+      <c r="E46" s="36" t="s">
+        <v>28</v>
       </c>
       <c r="F46" s="28"/>
       <c r="G46" s="14" t="s">
@@ -2429,45 +2361,75 @@
       </c>
       <c r="H46" s="28"/>
       <c r="I46" s="23" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="J46" s="41"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="33"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="7"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="42"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="42"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="42"/>
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="28"/>
+      <c r="G47" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="28"/>
+      <c r="I47" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J47" s="41"/>
+    </row>
+    <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="28"/>
+      <c r="G48" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="28"/>
+      <c r="I48" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J48" s="41"/>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="28"/>
+      <c r="G49" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="28"/>
+      <c r="I49" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J49" s="41"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
@@ -2529,31 +2491,76 @@
       <c r="I54" s="26"/>
       <c r="J54" s="42"/>
     </row>
-    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="6"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="25"/>
-      <c r="I55" s="27"/>
-      <c r="J55" s="43"/>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="24"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="24"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="42"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="24"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="24"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="24"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="42"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="24"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="42"/>
+    </row>
+    <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="27"/>
+      <c r="J58" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C33:D33"/>
+  <mergeCells count="46">
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="I5:J5"/>
@@ -2569,23 +2576,17 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C1:H2"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Inclusão da classe GETimer
Inclusão da classe GETimer
Atualização das classes GETimeHandler e Game Engine
Atualização dos documentos para Sprint #2
Atualização dos testes de unidade
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B16F260-442F-4791-A5D5-62EF2C4DC211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FE68F5-A73E-4466-A2DA-7187FF91F0C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="124">
   <si>
     <t>BPM Game Engine</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t>TimeHandler GameEngine</t>
+  </si>
+  <si>
+    <t>Utilizar um objeto GETimer</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GETimer e configurá-lo para terminar em 1 segundo.</t>
+  </si>
+  <si>
+    <t>TimeHandler</t>
   </si>
 </sst>
 </file>
@@ -940,167 +949,167 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,7 +1129,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1418,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:D35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,32 +1445,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="74"/>
+      <c r="C1" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="61"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="78"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="A2" s="75"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="80"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1469,60 +1478,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="73" t="s">
+      <c r="B5" s="99"/>
+      <c r="C5" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="81" t="s">
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="82"/>
-      <c r="I5" s="64" t="s">
+      <c r="H5" s="99"/>
+      <c r="I5" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="65"/>
+      <c r="J5" s="82"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="76" t="s">
+      <c r="B6" s="101"/>
+      <c r="C6" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="77"/>
-      <c r="E6" s="77"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="83" t="s">
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="84"/>
-      <c r="I6" s="66">
+      <c r="H6" s="101"/>
+      <c r="I6" s="83">
         <v>44046</v>
       </c>
-      <c r="J6" s="67"/>
+      <c r="J6" s="84"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="79" t="s">
+      <c r="B7" s="97"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="96" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="80"/>
-      <c r="I7" s="68"/>
-      <c r="J7" s="69"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="86"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1536,10 +1545,10 @@
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="88"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
@@ -1566,10 +1575,10 @@
       <c r="B12" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C12" s="89" t="s">
+      <c r="C12" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="90"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="36" t="s">
         <v>28</v>
       </c>
@@ -1596,10 +1605,10 @@
       <c r="B13" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="55"/>
+      <c r="D13" s="63"/>
       <c r="E13" s="37" t="s">
         <v>28</v>
       </c>
@@ -1626,10 +1635,10 @@
       <c r="B14" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="55"/>
+      <c r="D14" s="63"/>
       <c r="E14" s="37" t="s">
         <v>28</v>
       </c>
@@ -1656,10 +1665,10 @@
       <c r="B15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="55"/>
+      <c r="D15" s="63"/>
       <c r="E15" s="38" t="s">
         <v>54</v>
       </c>
@@ -1686,10 +1695,10 @@
       <c r="B16" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="55"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
@@ -1716,10 +1725,10 @@
       <c r="B17" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="37" t="s">
         <v>28</v>
       </c>
@@ -1744,10 +1753,10 @@
       <c r="B18" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="37" t="s">
         <v>32</v>
       </c>
@@ -1774,10 +1783,10 @@
       <c r="B19" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="55"/>
+      <c r="D19" s="63"/>
       <c r="E19" s="37" t="s">
         <v>32</v>
       </c>
@@ -1804,10 +1813,10 @@
       <c r="B20" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="D20" s="55"/>
+      <c r="D20" s="63"/>
       <c r="E20" s="37" t="s">
         <v>32</v>
       </c>
@@ -1834,10 +1843,10 @@
       <c r="B21" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="D21" s="93"/>
+      <c r="D21" s="66"/>
       <c r="E21" s="38" t="s">
         <v>35</v>
       </c>
@@ -1860,8 +1869,8 @@
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
       <c r="B22" s="46"/>
-      <c r="C22" s="91"/>
-      <c r="D22" s="92"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="72"/>
       <c r="E22" s="47"/>
       <c r="F22" s="48"/>
       <c r="G22" s="49"/>
@@ -1873,13 +1882,13 @@
       <c r="A23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="B23" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="D23" s="55"/>
+      <c r="D23" s="63"/>
       <c r="E23" s="37" t="s">
         <v>32</v>
       </c>
@@ -1904,10 +1913,10 @@
       <c r="B24" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="D24" s="55"/>
+      <c r="D24" s="63"/>
       <c r="E24" s="37" t="s">
         <v>32</v>
       </c>
@@ -1931,13 +1940,13 @@
       <c r="A25" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="94" t="s">
+      <c r="B25" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="D25" s="55"/>
+      <c r="D25" s="63"/>
       <c r="E25" s="38" t="s">
         <v>60</v>
       </c>
@@ -1957,23 +1966,41 @@
         <v>43891</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="95"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="40"/>
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="D26" s="63"/>
+      <c r="E26" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="40">
+        <v>43895</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="96"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="55"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="63"/>
       <c r="E27" s="37"/>
       <c r="F27" s="20"/>
       <c r="G27" s="13"/>
@@ -1983,9 +2010,9 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="63"/>
       <c r="E28" s="38"/>
       <c r="F28" s="20"/>
       <c r="G28" s="13"/>
@@ -1995,9 +2022,9 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="54"/>
-      <c r="D29" s="55"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="63"/>
       <c r="E29" s="38"/>
       <c r="F29" s="20"/>
       <c r="G29" s="13"/>
@@ -2006,16 +2033,16 @@
       <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="97"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="100"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="102"/>
-      <c r="H30" s="103"/>
-      <c r="I30" s="104"/>
-      <c r="J30" s="105"/>
+      <c r="A30" s="55"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="61"/>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -2024,10 +2051,10 @@
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="54" t="s">
+      <c r="C31" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="55"/>
+      <c r="D31" s="63"/>
       <c r="E31" s="38" t="s">
         <v>35</v>
       </c>
@@ -2049,9 +2076,9 @@
     </row>
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="55"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="63"/>
       <c r="E32" s="38"/>
       <c r="F32" s="20"/>
       <c r="G32" s="13"/>
@@ -2066,10 +2093,10 @@
       <c r="B33" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="55"/>
+      <c r="D33" s="63"/>
       <c r="E33" s="38" t="s">
         <v>60</v>
       </c>
@@ -2096,8 +2123,8 @@
       <c r="B34" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="53"/>
+      <c r="C34" s="104"/>
+      <c r="D34" s="105"/>
       <c r="E34" s="38" t="s">
         <v>32</v>
       </c>
@@ -2118,8 +2145,8 @@
       <c r="B35" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="52"/>
-      <c r="D35" s="53"/>
+      <c r="C35" s="104"/>
+      <c r="D35" s="105"/>
       <c r="E35" s="38" t="s">
         <v>63</v>
       </c>
@@ -2140,8 +2167,8 @@
       <c r="B36" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="53"/>
+      <c r="C36" s="104"/>
+      <c r="D36" s="105"/>
       <c r="E36" s="38" t="s">
         <v>66</v>
       </c>
@@ -2162,8 +2189,8 @@
       <c r="B37" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="53"/>
+      <c r="C37" s="104"/>
+      <c r="D37" s="105"/>
       <c r="E37" s="38" t="s">
         <v>68</v>
       </c>
@@ -2184,8 +2211,8 @@
       <c r="B38" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C38" s="52"/>
-      <c r="D38" s="53"/>
+      <c r="C38" s="104"/>
+      <c r="D38" s="105"/>
       <c r="E38" s="38" t="s">
         <v>70</v>
       </c>
@@ -2206,8 +2233,8 @@
       <c r="B39" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="53"/>
+      <c r="C39" s="104"/>
+      <c r="D39" s="105"/>
       <c r="E39" s="38" t="s">
         <v>74</v>
       </c>
@@ -2228,8 +2255,8 @@
       <c r="B40" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="52"/>
-      <c r="D40" s="53"/>
+      <c r="C40" s="104"/>
+      <c r="D40" s="105"/>
       <c r="E40" s="38" t="s">
         <v>76</v>
       </c>
@@ -2250,8 +2277,8 @@
       <c r="B41" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="52"/>
-      <c r="D41" s="53"/>
+      <c r="C41" s="104"/>
+      <c r="D41" s="105"/>
       <c r="E41" s="38" t="s">
         <v>32</v>
       </c>
@@ -2541,26 +2568,17 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="I5:J5"/>
@@ -2576,17 +2594,26 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C1:H2"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da demo para Sprint 2
Correções nas classes GEDiag e GameEngine
Inclusão de um novo teste de unidade
Atualização no documento Lista de Requisitos
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FE68F5-A73E-4466-A2DA-7187FF91F0C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B1A880-3267-44B7-A1CC-D98D39ED4D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="125">
   <si>
     <t>BPM Game Engine</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Calcular a quantidade de quadros por segundo</t>
   </si>
   <si>
-    <t>Obter o número de quadros executados por segundo.</t>
-  </si>
-  <si>
     <t>Sistema de Entidades</t>
   </si>
   <si>
@@ -403,6 +400,12 @@
   </si>
   <si>
     <t>TimeHandler</t>
+  </si>
+  <si>
+    <t>Utilizar um objeto da classe GEDiag para verificar a quantidade de quadros por segundo.</t>
+  </si>
+  <si>
+    <t>TimeHandler GEDiag</t>
   </si>
 </sst>
 </file>
@@ -980,11 +983,128 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -993,123 +1113,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1129,7 +1132,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1427,8 +1430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,32 +1448,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="73" t="s">
+      <c r="B1" s="67"/>
+      <c r="C1" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="71"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="75"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="80"/>
+      <c r="A2" s="68"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="73"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1478,60 +1481,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="90" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="98" t="s">
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="99"/>
-      <c r="I5" s="81" t="s">
+      <c r="H5" s="92"/>
+      <c r="I5" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="82"/>
+      <c r="J5" s="75"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="93" t="s">
+      <c r="B6" s="94"/>
+      <c r="C6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="100" t="s">
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="101"/>
-      <c r="I6" s="83">
+      <c r="H6" s="94"/>
+      <c r="I6" s="76">
         <v>44046</v>
       </c>
-      <c r="J6" s="84"/>
+      <c r="J6" s="77"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="97"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="96" t="s">
+      <c r="B7" s="90"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="97"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="86"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="79"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1545,10 +1548,10 @@
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="68"/>
+      <c r="D11" s="98"/>
       <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
@@ -1573,12 +1576,12 @@
         <v>14</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="70"/>
+      <c r="D12" s="100"/>
       <c r="E12" s="36" t="s">
         <v>28</v>
       </c>
@@ -1603,12 +1606,12 @@
         <v>15</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="63"/>
+      <c r="D13" s="65"/>
       <c r="E13" s="37" t="s">
         <v>28</v>
       </c>
@@ -1633,12 +1636,12 @@
         <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="63"/>
+      <c r="D14" s="65"/>
       <c r="E14" s="37" t="s">
         <v>28</v>
       </c>
@@ -1665,10 +1668,10 @@
       <c r="B15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="63"/>
+      <c r="D15" s="65"/>
       <c r="E15" s="38" t="s">
         <v>54</v>
       </c>
@@ -1693,12 +1696,12 @@
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="62" t="s">
-        <v>99</v>
-      </c>
-      <c r="D16" s="63"/>
+      <c r="D16" s="65"/>
       <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
@@ -1723,12 +1726,12 @@
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="D17" s="63"/>
+      <c r="D17" s="65"/>
       <c r="E17" s="37" t="s">
         <v>28</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>14</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I17" s="16" t="s">
         <v>30</v>
@@ -1748,15 +1751,15 @@
     </row>
     <row r="18" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="64" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="62" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="65"/>
       <c r="E18" s="37" t="s">
         <v>32</v>
       </c>
@@ -1778,15 +1781,15 @@
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C19" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="D19" s="63"/>
+      <c r="C19" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="65"/>
       <c r="E19" s="37" t="s">
         <v>32</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>14</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>30</v>
@@ -1811,12 +1814,12 @@
         <v>57</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C20" s="62" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="63"/>
+        <v>107</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="65"/>
       <c r="E20" s="37" t="s">
         <v>32</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>14</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>30</v>
@@ -1841,23 +1844,23 @@
         <v>20</v>
       </c>
       <c r="B21" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C21" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="C21" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="66"/>
+      <c r="D21" s="105"/>
       <c r="E21" s="38" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I21" s="16" t="s">
         <v>30</v>
@@ -1869,8 +1872,8 @@
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="45"/>
       <c r="B22" s="46"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="72"/>
+      <c r="C22" s="101"/>
+      <c r="D22" s="102"/>
       <c r="E22" s="47"/>
       <c r="F22" s="48"/>
       <c r="G22" s="49"/>
@@ -1883,12 +1886,12 @@
         <v>21</v>
       </c>
       <c r="B23" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="62" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="63"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="37" t="s">
         <v>32</v>
       </c>
@@ -1913,15 +1916,15 @@
       <c r="B24" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="63"/>
+      <c r="C24" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D24" s="65"/>
       <c r="E24" s="37" t="s">
         <v>32</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>15</v>
@@ -1941,17 +1944,17 @@
         <v>59</v>
       </c>
       <c r="B25" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="C25" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" s="63"/>
+      <c r="D25" s="65"/>
       <c r="E25" s="38" t="s">
         <v>60</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>15</v>
@@ -1971,17 +1974,17 @@
         <v>22</v>
       </c>
       <c r="B26" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="C26" s="62" t="s">
-        <v>122</v>
-      </c>
-      <c r="D26" s="63"/>
+      <c r="D26" s="65"/>
       <c r="E26" s="38" t="s">
         <v>60</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>15</v>
@@ -1996,23 +1999,41 @@
         <v>43895</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="40"/>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="D27" s="65"/>
+      <c r="E27" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I27" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="40">
+        <v>43902</v>
+      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="54"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="63"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="65"/>
       <c r="E28" s="38"/>
       <c r="F28" s="20"/>
       <c r="G28" s="13"/>
@@ -2023,8 +2044,8 @@
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="54"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="63"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
       <c r="E29" s="38"/>
       <c r="F29" s="20"/>
       <c r="G29" s="13"/>
@@ -2035,8 +2056,8 @@
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="55"/>
       <c r="B30" s="53"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="65"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="104"/>
       <c r="E30" s="56"/>
       <c r="F30" s="57"/>
       <c r="G30" s="58"/>
@@ -2051,10 +2072,10 @@
       <c r="B31" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="63"/>
+      <c r="D31" s="65"/>
       <c r="E31" s="38" t="s">
         <v>35</v>
       </c>
@@ -2077,8 +2098,8 @@
     <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12"/>
       <c r="B32" s="54"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="63"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="38"/>
       <c r="F32" s="20"/>
       <c r="G32" s="13"/>
@@ -2087,44 +2108,26 @@
       <c r="J32" s="40"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="62" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="63"/>
-      <c r="E33" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J33" s="40">
-        <v>43908</v>
-      </c>
+      <c r="A33" s="12"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="40"/>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="104"/>
-      <c r="D34" s="105"/>
+        <v>64</v>
+      </c>
+      <c r="C34" s="62"/>
+      <c r="D34" s="63"/>
       <c r="E34" s="38" t="s">
         <v>32</v>
       </c>
@@ -2134,7 +2137,7 @@
       </c>
       <c r="H34" s="14"/>
       <c r="I34" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J34" s="40"/>
     </row>
@@ -2143,12 +2146,12 @@
         <v>24</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="104"/>
-      <c r="D35" s="105"/>
+        <v>76</v>
+      </c>
+      <c r="C35" s="62"/>
+      <c r="D35" s="63"/>
       <c r="E35" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="13" t="s">
@@ -2156,7 +2159,7 @@
       </c>
       <c r="H35" s="14"/>
       <c r="I35" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J35" s="40"/>
     </row>
@@ -2165,12 +2168,12 @@
         <v>25</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="104"/>
-      <c r="D36" s="105"/>
+        <v>77</v>
+      </c>
+      <c r="C36" s="62"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="13" t="s">
@@ -2178,7 +2181,7 @@
       </c>
       <c r="H36" s="14"/>
       <c r="I36" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J36" s="40"/>
     </row>
@@ -2187,12 +2190,12 @@
         <v>26</v>
       </c>
       <c r="B37" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="62"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="38" t="s">
         <v>67</v>
-      </c>
-      <c r="C37" s="104"/>
-      <c r="D37" s="105"/>
-      <c r="E37" s="38" t="s">
-        <v>68</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="13" t="s">
@@ -2200,7 +2203,7 @@
       </c>
       <c r="H37" s="14"/>
       <c r="I37" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J37" s="40"/>
     </row>
@@ -2209,12 +2212,12 @@
         <v>27</v>
       </c>
       <c r="B38" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="62"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="38" t="s">
         <v>69</v>
-      </c>
-      <c r="C38" s="104"/>
-      <c r="D38" s="105"/>
-      <c r="E38" s="38" t="s">
-        <v>70</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="13" t="s">
@@ -2222,21 +2225,21 @@
       </c>
       <c r="H38" s="14"/>
       <c r="I38" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="104"/>
-      <c r="D39" s="105"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="63"/>
       <c r="E39" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F39" s="20"/>
       <c r="G39" s="13" t="s">
@@ -2244,21 +2247,21 @@
       </c>
       <c r="H39" s="14"/>
       <c r="I39" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J39" s="40"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="62"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="38" t="s">
         <v>75</v>
-      </c>
-      <c r="C40" s="104"/>
-      <c r="D40" s="105"/>
-      <c r="E40" s="38" t="s">
-        <v>76</v>
       </c>
       <c r="F40" s="20"/>
       <c r="G40" s="13" t="s">
@@ -2266,19 +2269,19 @@
       </c>
       <c r="H40" s="14"/>
       <c r="I40" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J40" s="40"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="104"/>
-      <c r="D41" s="105"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="63"/>
       <c r="E41" s="38" t="s">
         <v>32</v>
       </c>
@@ -2288,16 +2291,16 @@
       </c>
       <c r="H41" s="14"/>
       <c r="I41" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J41" s="40"/>
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C42" s="28"/>
       <c r="D42" s="28"/>
@@ -2310,16 +2313,16 @@
       </c>
       <c r="H42" s="28"/>
       <c r="I42" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J42" s="41"/>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
@@ -2332,7 +2335,7 @@
       </c>
       <c r="H43" s="28"/>
       <c r="I43" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J43" s="41"/>
     </row>
@@ -2350,10 +2353,10 @@
     </row>
     <row r="45" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C45" s="28"/>
       <c r="D45" s="28"/>
@@ -2366,16 +2369,16 @@
       </c>
       <c r="H45" s="28"/>
       <c r="I45" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
@@ -2388,16 +2391,16 @@
       </c>
       <c r="H46" s="28"/>
       <c r="I46" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J46" s="41"/>
     </row>
     <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" s="29" t="s">
         <v>89</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>90</v>
       </c>
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
@@ -2410,16 +2413,16 @@
       </c>
       <c r="H47" s="28"/>
       <c r="I47" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J47" s="41"/>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C48" s="28"/>
       <c r="D48" s="28"/>
@@ -2432,16 +2435,16 @@
       </c>
       <c r="H48" s="28"/>
       <c r="I48" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J48" s="41"/>
     </row>
     <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C49" s="28"/>
       <c r="D49" s="28"/>
@@ -2454,7 +2457,7 @@
       </c>
       <c r="H49" s="28"/>
       <c r="I49" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J49" s="41"/>
     </row>
@@ -2568,17 +2571,26 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="I5:J5"/>
@@ -2594,26 +2606,17 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C1:H2"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização dos documentos finalizados para Sprint 2
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B1A880-3267-44B7-A1CC-D98D39ED4D42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D336E66-B8C5-448F-8453-503C6A50F9D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="132">
   <si>
     <t>BPM Game Engine</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Gerenciador de Tempo</t>
   </si>
   <si>
-    <t>Calcular a quantidade de quadros por segundo</t>
-  </si>
-  <si>
     <t>Sistema de Entidades</t>
   </si>
   <si>
@@ -297,24 +294,12 @@
     <t>#28</t>
   </si>
   <si>
-    <t>#29</t>
-  </si>
-  <si>
-    <t>Instanciar um objeto Timer</t>
-  </si>
-  <si>
     <t>Inclusão de Frame Rate Governing</t>
   </si>
   <si>
-    <t>Implementação da classe Timer</t>
-  </si>
-  <si>
     <t>#30</t>
   </si>
   <si>
-    <t>#31</t>
-  </si>
-  <si>
     <t>Instanciar uma janela de aplicação</t>
   </si>
   <si>
@@ -406,6 +391,42 @@
   </si>
   <si>
     <t>TimeHandler GEDiag</t>
+  </si>
+  <si>
+    <t>Obter o tempo a partir do registrador High-Res-Timer</t>
+  </si>
+  <si>
+    <t>Obter a quantidade de ciclos executados desde o momento que o processador foi iniciado a partir do registrador High-Resolution-Timer e obter também a frequência de ciclos por segundo a partir do registrador High-Resolution-Timer.</t>
+  </si>
+  <si>
+    <t>High-Resolution-Timer</t>
+  </si>
+  <si>
+    <t>Calcular e obter a quantidade de quadros por segundo</t>
+  </si>
+  <si>
+    <t>Configurar a viewport do sistema de renderização</t>
+  </si>
+  <si>
+    <t>Utilizar um objeto da classe GERenderingSystem para configurar a viewport (OpenGL) de renderização.</t>
+  </si>
+  <si>
+    <t>#18</t>
+  </si>
+  <si>
+    <t>Alteração da cor de fundo da janela de aplicação</t>
+  </si>
+  <si>
+    <t>Utilizar o sistema de renderização para alterar a cor de fundo da janela de aplicação.</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe Diagnostico</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe Diag e inicializá-lo com um objeto TimeHandler</t>
+  </si>
+  <si>
+    <t>Diagnostico</t>
   </si>
 </sst>
 </file>
@@ -464,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,12 +501,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -817,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -880,9 +895,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -893,16 +905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -935,184 +938,208 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1430,8 +1457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,32 +1475,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="66" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="71"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="68"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="73"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="97"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="74"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1481,60 +1508,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="91" t="s">
+      <c r="A5" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="83" t="s">
+      <c r="B5" s="93"/>
+      <c r="C5" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="91" t="s">
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="92"/>
-      <c r="I5" s="74" t="s">
+      <c r="H5" s="93"/>
+      <c r="I5" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="75"/>
+      <c r="J5" s="76"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="94"/>
-      <c r="C6" s="86" t="s">
+      <c r="B6" s="95"/>
+      <c r="C6" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="93" t="s">
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="94"/>
-      <c r="I6" s="76">
+      <c r="H6" s="95"/>
+      <c r="I6" s="77">
         <v>44046</v>
       </c>
-      <c r="J6" s="77"/>
+      <c r="J6" s="78"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="90"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="89" t="s">
+      <c r="B7" s="91"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="90"/>
-      <c r="I7" s="78"/>
-      <c r="J7" s="79"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="79"/>
+      <c r="J7" s="80"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1548,10 +1575,10 @@
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="98"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="2" t="s">
         <v>39</v>
       </c>
@@ -1576,16 +1603,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="100"/>
-      <c r="E12" s="36" t="s">
+      <c r="D12" s="64"/>
+      <c r="E12" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="31" t="s">
         <v>47</v>
       </c>
       <c r="G12" s="10" t="s">
@@ -1597,7 +1624,7 @@
       <c r="I12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="39">
+      <c r="J12" s="35">
         <v>43879</v>
       </c>
     </row>
@@ -1606,13 +1633,13 @@
         <v>15</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="64" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="65"/>
-      <c r="E13" s="37" t="s">
+      <c r="D13" s="57"/>
+      <c r="E13" s="33" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="20" t="s">
@@ -1627,7 +1654,7 @@
       <c r="I13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="36">
         <v>43877</v>
       </c>
     </row>
@@ -1636,13 +1663,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="64" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="37" t="s">
+      <c r="D14" s="57"/>
+      <c r="E14" s="33" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="20" t="s">
@@ -1657,7 +1684,7 @@
       <c r="I14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="40">
+      <c r="J14" s="36">
         <v>43879</v>
       </c>
     </row>
@@ -1668,11 +1695,11 @@
       <c r="B15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="38" t="s">
+      <c r="D15" s="57"/>
+      <c r="E15" s="34" t="s">
         <v>54</v>
       </c>
       <c r="F15" s="20" t="s">
@@ -1687,7 +1714,7 @@
       <c r="I15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="40">
+      <c r="J15" s="36">
         <v>43881</v>
       </c>
     </row>
@@ -1696,13 +1723,13 @@
         <v>18</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="64" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" s="65"/>
-      <c r="E16" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="57"/>
+      <c r="E16" s="34" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="20" t="s">
@@ -1717,7 +1744,7 @@
       <c r="I16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J16" s="40">
+      <c r="J16" s="36">
         <v>43880</v>
       </c>
     </row>
@@ -1726,13 +1753,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="64" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" s="33" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="20"/>
@@ -1740,27 +1767,27 @@
         <v>14</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="40">
+      <c r="J17" s="36">
         <v>43880</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="64" t="s">
-        <v>104</v>
-      </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="57"/>
+      <c r="E18" s="33" t="s">
         <v>32</v>
       </c>
       <c r="F18" s="20" t="s">
@@ -1775,22 +1802,22 @@
       <c r="I18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="40">
+      <c r="J18" s="36">
         <v>43886</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="57"/>
+      <c r="E19" s="33" t="s">
         <v>32</v>
       </c>
       <c r="F19" s="20" t="s">
@@ -1800,12 +1827,12 @@
         <v>14</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I19" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J19" s="40">
+      <c r="J19" s="36">
         <v>43882</v>
       </c>
     </row>
@@ -1814,13 +1841,13 @@
         <v>57</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="D20" s="65"/>
-      <c r="E20" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="57"/>
+      <c r="E20" s="33" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="20" t="s">
@@ -1830,12 +1857,12 @@
         <v>14</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="40">
+      <c r="J20" s="36">
         <v>43884</v>
       </c>
     </row>
@@ -1843,56 +1870,56 @@
       <c r="A21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="C21" s="64" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="105"/>
-      <c r="E21" s="38" t="s">
+      <c r="B21" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="60"/>
+      <c r="E21" s="34" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="I21" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J21" s="40">
+      <c r="J21" s="36">
         <v>43885</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="46"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="102"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="51"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="47"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="52" t="s">
-        <v>113</v>
-      </c>
-      <c r="C23" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="37" t="s">
+      <c r="B23" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="57"/>
+      <c r="E23" s="33" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="20"/>
@@ -1905,26 +1932,26 @@
       <c r="I23" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J23" s="40">
-        <v>43890</v>
+      <c r="J23" s="36">
+        <v>43921</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="37" t="s">
+      <c r="C24" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="57"/>
+      <c r="E24" s="33" t="s">
         <v>32</v>
       </c>
       <c r="F24" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>15</v>
@@ -1935,26 +1962,26 @@
       <c r="I24" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J24" s="40">
-        <v>43890</v>
+      <c r="J24" s="36">
+        <v>43921</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="65"/>
-      <c r="E25" s="38" t="s">
+      <c r="B25" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="57"/>
+      <c r="E25" s="34" t="s">
         <v>60</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>15</v>
@@ -1965,26 +1992,26 @@
       <c r="I25" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J25" s="40">
-        <v>43891</v>
+      <c r="J25" s="36">
+        <v>43902</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="D26" s="65"/>
-      <c r="E26" s="38" t="s">
+      <c r="B26" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="57"/>
+      <c r="E26" s="34" t="s">
         <v>60</v>
       </c>
       <c r="F26" s="20" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>15</v>
@@ -1995,7 +2022,7 @@
       <c r="I26" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="40">
+      <c r="J26" s="36">
         <v>43895</v>
       </c>
     </row>
@@ -2003,18 +2030,18 @@
       <c r="A27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="65"/>
-      <c r="E27" s="37" t="s">
+      <c r="C27" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="57"/>
+      <c r="E27" s="33" t="s">
         <v>32</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G27" s="13" t="s">
         <v>15</v>
@@ -2025,65 +2052,115 @@
       <c r="I27" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J27" s="40">
+      <c r="J27" s="36">
         <v>43902</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="65"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="40"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="38"/>
+    <row r="28" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="57"/>
+      <c r="E28" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="36">
+        <v>43907</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="57"/>
+      <c r="E29" s="34" t="s">
+        <v>35</v>
+      </c>
       <c r="F29" s="20"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="40"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="103"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="61"/>
+      <c r="G29" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" s="36">
+        <v>43885</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C30" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="59"/>
+      <c r="E30" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="51"/>
+      <c r="G30" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="J30" s="55">
+        <v>43903</v>
+      </c>
     </row>
     <row r="31" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="65"/>
-      <c r="E31" s="38" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="57"/>
+      <c r="E31" s="34" t="s">
+        <v>131</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>49</v>
+        <v>117</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H31" s="14" t="s">
         <v>31</v>
@@ -2091,44 +2168,44 @@
       <c r="I31" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="40" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="40"/>
+      <c r="J31" s="36">
+        <v>43902</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="41"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="100"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="102"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="104"/>
+      <c r="J32" s="105"/>
     </row>
     <row r="33" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="38"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="34"/>
       <c r="F33" s="20"/>
       <c r="G33" s="13"/>
       <c r="H33" s="14"/>
       <c r="I33" s="16"/>
-      <c r="J33" s="40"/>
+      <c r="J33" s="36"/>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="38" t="s">
+      <c r="B34" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="98"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="34" t="s">
         <v>32</v>
       </c>
       <c r="F34" s="20"/>
@@ -2136,153 +2213,153 @@
         <v>16</v>
       </c>
       <c r="H34" s="14"/>
-      <c r="I34" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J34" s="40"/>
+      <c r="I34" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J34" s="36"/>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="38" t="s">
-        <v>62</v>
+      <c r="B35" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="98"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="34" t="s">
+        <v>61</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H35" s="14"/>
-      <c r="I35" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" s="40"/>
+      <c r="I35" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J35" s="36"/>
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="62"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="38" t="s">
-        <v>65</v>
+      <c r="B36" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="98"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H36" s="14"/>
-      <c r="I36" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J36" s="40"/>
+      <c r="I36" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J36" s="36"/>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="98"/>
+      <c r="D37" s="99"/>
+      <c r="E37" s="34" t="s">
         <v>66</v>
-      </c>
-      <c r="C37" s="62"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="38" t="s">
-        <v>67</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H37" s="14"/>
-      <c r="I37" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J37" s="40"/>
+      <c r="I37" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B38" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="98"/>
+      <c r="D38" s="99"/>
+      <c r="E38" s="34" t="s">
         <v>68</v>
-      </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="38" t="s">
-        <v>69</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H38" s="14"/>
-      <c r="I38" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J38" s="40"/>
+      <c r="I38" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="62"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="38" t="s">
-        <v>73</v>
+      <c r="C39" s="98"/>
+      <c r="D39" s="99"/>
+      <c r="E39" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="F39" s="20"/>
       <c r="G39" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H39" s="14"/>
-      <c r="I39" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J39" s="40"/>
+      <c r="I39" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J39" s="36"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="98"/>
+      <c r="D40" s="99"/>
+      <c r="E40" s="34" t="s">
         <v>74</v>
-      </c>
-      <c r="C40" s="62"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="38" t="s">
-        <v>75</v>
       </c>
       <c r="F40" s="20"/>
       <c r="G40" s="13" t="s">
         <v>16</v>
       </c>
       <c r="H40" s="14"/>
-      <c r="I40" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J40" s="40"/>
+      <c r="I40" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J40" s="36"/>
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="38" t="s">
+      <c r="C41" s="98"/>
+      <c r="D41" s="99"/>
+      <c r="E41" s="34" t="s">
         <v>32</v>
       </c>
       <c r="F41" s="20"/>
@@ -2290,307 +2367,297 @@
         <v>16</v>
       </c>
       <c r="H41" s="14"/>
-      <c r="I41" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J41" s="40"/>
+      <c r="I41" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J41" s="36"/>
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="28"/>
+      <c r="F42" s="27"/>
       <c r="G42" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="28"/>
-      <c r="I42" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J42" s="41"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J42" s="37"/>
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="106" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="28"/>
+      <c r="F43" s="27"/>
       <c r="G43" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H43" s="28"/>
-      <c r="I43" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J43" s="41"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J43" s="37"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="28"/>
+      <c r="B44" s="106"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="27"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="37"/>
     </row>
     <row r="45" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="106" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F45" s="28"/>
+      <c r="F45" s="27"/>
       <c r="G45" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H45" s="28"/>
-      <c r="I45" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J45" s="41"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J45" s="37"/>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="106" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="28"/>
+      <c r="F46" s="27"/>
       <c r="G46" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H46" s="28"/>
-      <c r="I46" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J46" s="41"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="28"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="F47" s="28"/>
-      <c r="G47" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="28"/>
-      <c r="I47" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J47" s="41"/>
+      <c r="A47" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="57"/>
+      <c r="E47" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="F47" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J47" s="36" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B48" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="F48" s="28"/>
+      <c r="F48" s="27"/>
       <c r="G48" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="28"/>
-      <c r="I48" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J48" s="41"/>
-    </row>
-    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C49" s="28"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="F49" s="28"/>
-      <c r="G49" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H49" s="28"/>
-      <c r="I49" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J49" s="41"/>
+      <c r="H48" s="27"/>
+      <c r="I48" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J48" s="37"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="106"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="27"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="37"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="24"/>
+      <c r="B50" s="107"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="23"/>
       <c r="G50" s="7"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="26"/>
-      <c r="J50" s="42"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="38"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
-      <c r="B51" s="30"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="24"/>
+      <c r="B51" s="107"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="23"/>
       <c r="G51" s="7"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="42"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="38"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
-      <c r="B52" s="30"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="24"/>
+      <c r="B52" s="107"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="23"/>
       <c r="G52" s="7"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="42"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="38"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="24"/>
+      <c r="B53" s="107"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="23"/>
       <c r="G53" s="7"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="42"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="38"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="24"/>
+      <c r="B54" s="107"/>
+      <c r="C54" s="23"/>
+      <c r="D54" s="23"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="23"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="42"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="38"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="24"/>
+      <c r="B55" s="107"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="23"/>
       <c r="G55" s="7"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="42"/>
+      <c r="H55" s="23"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="38"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="24"/>
+      <c r="B56" s="107"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="23"/>
       <c r="G56" s="7"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="26"/>
-      <c r="J56" s="42"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="25"/>
+      <c r="J56" s="38"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
-      <c r="B57" s="30"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="24"/>
+      <c r="B57" s="107"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="23"/>
       <c r="G57" s="7"/>
-      <c r="H57" s="24"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="42"/>
+      <c r="H57" s="23"/>
+      <c r="I57" s="25"/>
+      <c r="J57" s="38"/>
     </row>
     <row r="58" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="25"/>
+      <c r="B58" s="108"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="24"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="27"/>
-      <c r="J58" s="43"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C22:D22"/>
+  <mergeCells count="47">
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="I5:J5"/>
@@ -2606,17 +2673,26 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C1:H2"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Correções de bugs, revisão de código e refatoração
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458193AD-CCEC-4813-92D3-5F465ECF3CBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F5E5E9-0F69-49E1-B489-80C54AD10F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -161,18 +161,9 @@
     <t>DATA</t>
   </si>
   <si>
-    <t>Instanciar um objeto da classe GEWindow e configurar todos os seus atributos.</t>
-  </si>
-  <si>
-    <t>Criar uma janela de aplicação no Microsoft Windows com um objeto GEWindow.</t>
-  </si>
-  <si>
     <t>ApiWrapper</t>
   </si>
   <si>
-    <t>Destruir uma janela de aplicação no Microsoft Windows utilizando a classe Window.</t>
-  </si>
-  <si>
     <t>ApiWrapper WinApiWrapper</t>
   </si>
   <si>
@@ -248,15 +239,6 @@
     <t>#30</t>
   </si>
   <si>
-    <t>Instanciar uma janela de aplicação</t>
-  </si>
-  <si>
-    <t>Criar uma janela de aplicação (Windows)</t>
-  </si>
-  <si>
-    <t>Destruir uma janela de aplicação (Windows)</t>
-  </si>
-  <si>
     <t>Exibir uma janela de aplicação na tela</t>
   </si>
   <si>
@@ -525,6 +507,24 @@
   </si>
   <si>
     <t>Obter dados de entrada a partir de um joystick</t>
+  </si>
+  <si>
+    <t>Criar uma janela de aplicação Windows</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GEWindowSystem</t>
+  </si>
+  <si>
+    <t>Instanciar um objeto da classe GEWindowSystem, validar os valores padrão (construtor) e reconfigurar todos os seus atributos.</t>
+  </si>
+  <si>
+    <t>Criar uma janela de aplicação no Microsoft Windows com um objeto GEWindowSystem.</t>
+  </si>
+  <si>
+    <t>Destruir uma janela de aplicação Windows</t>
+  </si>
+  <si>
+    <t>Destruir uma janela de aplicação no Microsoft Windows utilizando a classe GEWindowSystem.</t>
   </si>
 </sst>
 </file>
@@ -1091,150 +1091,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1252,20 +1108,164 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37:D37"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,32 +1601,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="62" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="67"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="77"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="69"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1634,60 +1634,60 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="79" t="s">
+      <c r="B5" s="98"/>
+      <c r="C5" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="87" t="s">
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="88"/>
-      <c r="I5" s="70" t="s">
+      <c r="H5" s="98"/>
+      <c r="I5" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="71"/>
+      <c r="J5" s="81"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="82" t="s">
+      <c r="B6" s="100"/>
+      <c r="C6" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="89" t="s">
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="90"/>
-      <c r="I6" s="72">
+      <c r="H6" s="100"/>
+      <c r="I6" s="82">
         <v>44046</v>
       </c>
-      <c r="J6" s="73"/>
+      <c r="J6" s="83"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="86"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
-      <c r="F7" s="78"/>
-      <c r="G7" s="85" t="s">
+      <c r="B7" s="96"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="86"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="75"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="85"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -1701,10 +1701,10 @@
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="56" t="s">
+      <c r="C11" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="57"/>
+      <c r="D11" s="67"/>
       <c r="E11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1729,17 +1729,17 @@
         <v>14</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="59"/>
+        <v>159</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="69"/>
       <c r="E12" s="23" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>14</v>
@@ -1759,17 +1759,17 @@
         <v>15</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="52"/>
+        <v>158</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" s="62"/>
       <c r="E13" s="24" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>14</v>
@@ -1789,17 +1789,17 @@
         <v>16</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="52"/>
+        <v>162</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" s="62"/>
       <c r="E14" s="24" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>14</v>
@@ -1819,17 +1819,17 @@
         <v>17</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="62"/>
+      <c r="E15" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>52</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>14</v>
@@ -1849,17 +1849,17 @@
         <v>18</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="52"/>
+        <v>68</v>
+      </c>
+      <c r="C16" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="62"/>
       <c r="E16" s="25" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>14</v>
@@ -1879,12 +1879,12 @@
         <v>19</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="52"/>
+        <v>70</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="62"/>
       <c r="E17" s="24" t="s">
         <v>28</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>14</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>30</v>
@@ -1904,20 +1904,20 @@
     </row>
     <row r="18" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="52"/>
+        <v>74</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="62"/>
       <c r="E18" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>14</v>
@@ -1934,26 +1934,26 @@
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" s="51" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="52"/>
+        <v>77</v>
+      </c>
+      <c r="C19" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="62"/>
       <c r="E19" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>30</v>
@@ -1964,26 +1964,26 @@
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="52"/>
+        <v>78</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="62"/>
       <c r="E20" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I20" s="13" t="s">
         <v>30</v>
@@ -1997,23 +1997,23 @@
         <v>20</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="55"/>
+        <v>81</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="65"/>
       <c r="E21" s="25" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>14</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>30</v>
@@ -2025,8 +2025,8 @@
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="31"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="71"/>
       <c r="E22" s="32"/>
       <c r="F22" s="33"/>
       <c r="G22" s="34"/>
@@ -2039,12 +2039,12 @@
         <v>21</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="C23" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="D23" s="52"/>
+        <v>84</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="62"/>
       <c r="E23" s="24" t="s">
         <v>32</v>
       </c>
@@ -2064,20 +2064,20 @@
     </row>
     <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="52"/>
+        <v>45</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="62"/>
       <c r="E24" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>15</v>
@@ -2094,20 +2094,20 @@
     </row>
     <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" s="52"/>
+        <v>88</v>
+      </c>
+      <c r="C25" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="62"/>
       <c r="E25" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>15</v>
@@ -2127,17 +2127,17 @@
         <v>22</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="52"/>
+        <v>91</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="62"/>
       <c r="E26" s="25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>15</v>
@@ -2157,17 +2157,17 @@
         <v>23</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="51" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="52"/>
+        <v>99</v>
+      </c>
+      <c r="C27" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" s="62"/>
       <c r="E27" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>15</v>
@@ -2187,17 +2187,17 @@
         <v>24</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28" s="51" t="s">
-        <v>103</v>
-      </c>
-      <c r="D28" s="52"/>
+        <v>96</v>
+      </c>
+      <c r="C28" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="62"/>
       <c r="E28" s="25" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>15</v>
@@ -2217,12 +2217,12 @@
         <v>25</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="D29" s="52"/>
+        <v>100</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="62"/>
       <c r="E29" s="25" t="s">
         <v>33</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>15</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>30</v>
@@ -2242,15 +2242,15 @@
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="53" t="s">
-        <v>110</v>
-      </c>
-      <c r="D30" s="54"/>
+        <v>103</v>
+      </c>
+      <c r="C30" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="64"/>
       <c r="E30" s="25" t="s">
         <v>33</v>
       </c>
@@ -2273,17 +2273,17 @@
         <v>26</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="51" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" s="52"/>
+        <v>105</v>
+      </c>
+      <c r="C31" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="62"/>
       <c r="E31" s="25" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>15</v>
@@ -2301,8 +2301,8 @@
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="50"/>
-      <c r="C32" s="94"/>
-      <c r="D32" s="95"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="32"/>
       <c r="F32" s="45"/>
       <c r="G32" s="46"/>
@@ -2314,13 +2314,13 @@
       <c r="A33" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="99" t="s">
-        <v>114</v>
-      </c>
-      <c r="C33" s="51" t="s">
-        <v>115</v>
-      </c>
-      <c r="D33" s="52"/>
+      <c r="B33" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="62"/>
       <c r="E33" s="25" t="s">
         <v>33</v>
       </c>
@@ -2338,24 +2338,24 @@
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="99" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="D34" s="55"/>
+        <v>58</v>
+      </c>
+      <c r="B34" s="51" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="65"/>
       <c r="E34" s="25" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="10" t="s">
         <v>16</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I34" s="13" t="s">
         <v>30</v>
@@ -2364,17 +2364,17 @@
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="99" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="D35" s="55"/>
+        <v>59</v>
+      </c>
+      <c r="B35" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="61" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="65"/>
       <c r="E35" s="25" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="10" t="s">
@@ -2390,20 +2390,20 @@
     </row>
     <row r="36" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="99" t="s">
-        <v>122</v>
-      </c>
-      <c r="C36" s="51" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="55"/>
+        <v>61</v>
+      </c>
+      <c r="B36" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="D36" s="65"/>
       <c r="E36" s="25" t="s">
         <v>28</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G36" s="10" t="s">
         <v>16</v>
@@ -2418,17 +2418,17 @@
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="99" t="s">
-        <v>124</v>
-      </c>
-      <c r="C37" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="D37" s="55"/>
+        <v>63</v>
+      </c>
+      <c r="B37" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="65"/>
       <c r="E37" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="10" t="s">
@@ -2444,17 +2444,17 @@
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="99" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="D38" s="52"/>
+        <v>64</v>
+      </c>
+      <c r="B38" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="61" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="62"/>
       <c r="E38" s="25" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="10" t="s">
@@ -2470,17 +2470,17 @@
     </row>
     <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" s="99" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="51" t="s">
-        <v>130</v>
-      </c>
-      <c r="D39" s="52"/>
+        <v>121</v>
+      </c>
+      <c r="B39" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="62"/>
       <c r="E39" s="25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="10" t="s">
@@ -2490,23 +2490,23 @@
         <v>29</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J39" s="27"/>
     </row>
     <row r="40" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="99" t="s">
-        <v>132</v>
-      </c>
-      <c r="C40" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40" s="52"/>
+        <v>65</v>
+      </c>
+      <c r="B40" s="51" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="62"/>
       <c r="E40" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="10" t="s">
@@ -2522,17 +2522,17 @@
     </row>
     <row r="41" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="99" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="D41" s="52"/>
+        <v>66</v>
+      </c>
+      <c r="B41" s="51" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="62"/>
       <c r="E41" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="10" t="s">
@@ -2549,8 +2549,8 @@
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="50"/>
-      <c r="C42" s="97"/>
-      <c r="D42" s="98"/>
+      <c r="C42" s="105"/>
+      <c r="D42" s="106"/>
       <c r="E42" s="32"/>
       <c r="F42" s="45"/>
       <c r="G42" s="46"/>
@@ -2560,15 +2560,15 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="C43" s="93"/>
-      <c r="D43" s="96"/>
+        <v>131</v>
+      </c>
+      <c r="C43" s="107"/>
+      <c r="D43" s="108"/>
       <c r="E43" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="10"/>
@@ -2580,15 +2580,15 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="C44" s="93"/>
-      <c r="D44" s="96"/>
+        <v>132</v>
+      </c>
+      <c r="C44" s="107"/>
+      <c r="D44" s="108"/>
       <c r="E44" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="10"/>
@@ -2600,13 +2600,13 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B45" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="93"/>
-      <c r="D45" s="96"/>
+        <v>62</v>
+      </c>
+      <c r="C45" s="107"/>
+      <c r="D45" s="108"/>
       <c r="E45" s="25" t="s">
         <v>32</v>
       </c>
@@ -2614,19 +2614,19 @@
       <c r="G45" s="10"/>
       <c r="H45" s="11"/>
       <c r="I45" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="C46" s="106"/>
-      <c r="D46" s="107"/>
+        <v>135</v>
+      </c>
+      <c r="C46" s="109"/>
+      <c r="D46" s="110"/>
       <c r="E46" s="25" t="s">
         <v>28</v>
       </c>
@@ -2634,39 +2634,39 @@
       <c r="G46" s="11"/>
       <c r="H46" s="20"/>
       <c r="I46" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J46" s="28"/>
     </row>
     <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B47" s="105" t="s">
-        <v>143</v>
-      </c>
-      <c r="C47" s="106"/>
-      <c r="D47" s="107"/>
+        <v>136</v>
+      </c>
+      <c r="B47" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="109"/>
+      <c r="D47" s="110"/>
       <c r="E47" s="25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="11"/>
       <c r="H47" s="20"/>
       <c r="I47" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J47" s="28"/>
     </row>
     <row r="48" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B48" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="106"/>
-      <c r="D48" s="107"/>
+        <v>139</v>
+      </c>
+      <c r="C48" s="109"/>
+      <c r="D48" s="110"/>
       <c r="E48" s="25" t="s">
         <v>28</v>
       </c>
@@ -2674,19 +2674,19 @@
       <c r="G48" s="11"/>
       <c r="H48" s="20"/>
       <c r="I48" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J48" s="28"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="C49" s="106"/>
-      <c r="D49" s="107"/>
+        <v>141</v>
+      </c>
+      <c r="C49" s="109"/>
+      <c r="D49" s="110"/>
       <c r="E49" s="25" t="s">
         <v>28</v>
       </c>
@@ -2694,99 +2694,99 @@
       <c r="G49" s="11"/>
       <c r="H49" s="20"/>
       <c r="I49" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J49" s="28"/>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="100" t="s">
-        <v>148</v>
-      </c>
-      <c r="B50" s="101" t="s">
-        <v>149</v>
-      </c>
-      <c r="C50" s="106" t="s">
-        <v>150</v>
-      </c>
-      <c r="D50" s="107"/>
-      <c r="E50" s="109" t="s">
+      <c r="A50" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="109" t="s">
+        <v>144</v>
+      </c>
+      <c r="D50" s="110"/>
+      <c r="E50" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="F50" s="102"/>
-      <c r="G50" s="103"/>
-      <c r="H50" s="102"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="54"/>
       <c r="I50" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J50" s="104"/>
+        <v>56</v>
+      </c>
+      <c r="J50" s="56"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B51" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" s="51"/>
-      <c r="D51" s="55"/>
+        <v>146</v>
+      </c>
+      <c r="C51" s="61"/>
+      <c r="D51" s="65"/>
       <c r="E51" s="25"/>
       <c r="F51" s="17"/>
       <c r="G51" s="10"/>
       <c r="H51" s="11"/>
       <c r="I51" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J51" s="27"/>
     </row>
     <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B52" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="C52" s="108"/>
-      <c r="D52" s="108"/>
+        <v>148</v>
+      </c>
+      <c r="C52" s="58"/>
+      <c r="D52" s="58"/>
       <c r="E52" s="25" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F52" s="20"/>
       <c r="G52" s="11"/>
       <c r="H52" s="20"/>
       <c r="I52" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J52" s="28"/>
     </row>
     <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B53" s="49" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" s="108"/>
-      <c r="D53" s="108"/>
+        <v>150</v>
+      </c>
+      <c r="C53" s="58"/>
+      <c r="D53" s="58"/>
       <c r="E53" s="25" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="11"/>
       <c r="H53" s="20"/>
       <c r="I53" s="19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J53" s="28"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" s="93"/>
-      <c r="D54" s="96"/>
+        <v>153</v>
+      </c>
+      <c r="C54" s="107"/>
+      <c r="D54" s="108"/>
       <c r="E54" s="25"/>
       <c r="F54" s="17"/>
       <c r="G54" s="10"/>
@@ -2796,13 +2796,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B55" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="C55" s="93"/>
-      <c r="D55" s="96"/>
+        <v>155</v>
+      </c>
+      <c r="C55" s="107"/>
+      <c r="D55" s="108"/>
       <c r="E55" s="25"/>
       <c r="F55" s="17"/>
       <c r="G55" s="10"/>
@@ -2812,13 +2812,13 @@
     </row>
     <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="C56" s="93"/>
-      <c r="D56" s="96"/>
+        <v>157</v>
+      </c>
+      <c r="C56" s="107"/>
+      <c r="D56" s="108"/>
       <c r="E56" s="25"/>
       <c r="F56" s="17"/>
       <c r="G56" s="10"/>
@@ -2829,8 +2829,8 @@
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="49"/>
-      <c r="C57" s="108"/>
-      <c r="D57" s="108"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="58"/>
       <c r="E57" s="25"/>
       <c r="F57" s="20"/>
       <c r="G57" s="11"/>
@@ -2841,8 +2841,8 @@
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="49"/>
-      <c r="C58" s="108"/>
-      <c r="D58" s="108"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="58"/>
       <c r="E58" s="25"/>
       <c r="F58" s="20"/>
       <c r="G58" s="11"/>
@@ -2853,8 +2853,8 @@
     <row r="59" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="9"/>
       <c r="B59" s="49"/>
-      <c r="C59" s="108"/>
-      <c r="D59" s="108"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="58"/>
       <c r="E59" s="25"/>
       <c r="F59" s="20"/>
       <c r="G59" s="11"/>
@@ -2865,9 +2865,9 @@
     <row r="60" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9"/>
       <c r="B60" s="49"/>
-      <c r="C60" s="108"/>
-      <c r="D60" s="108"/>
-      <c r="E60" s="110"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="58"/>
+      <c r="E60" s="60"/>
       <c r="F60" s="20"/>
       <c r="G60" s="11"/>
       <c r="H60" s="20"/>
@@ -2877,9 +2877,9 @@
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
       <c r="B61" s="49"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="108"/>
-      <c r="E61" s="110"/>
+      <c r="C61" s="58"/>
+      <c r="D61" s="58"/>
+      <c r="E61" s="60"/>
       <c r="F61" s="20"/>
       <c r="G61" s="11"/>
       <c r="H61" s="20"/>
@@ -2889,8 +2889,8 @@
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="38"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="55"/>
+      <c r="C62" s="61"/>
+      <c r="D62" s="65"/>
       <c r="E62" s="25"/>
       <c r="F62" s="17"/>
       <c r="G62" s="10"/>
@@ -2901,8 +2901,8 @@
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="9"/>
       <c r="B63" s="49"/>
-      <c r="C63" s="108"/>
-      <c r="D63" s="108"/>
+      <c r="C63" s="58"/>
+      <c r="D63" s="58"/>
       <c r="E63" s="25"/>
       <c r="F63" s="20"/>
       <c r="G63" s="11"/>

</xml_diff>

<commit_message>
Refatoração dos testes de unidade - CI
</commit_message>
<xml_diff>
--- a/docs/Lista de Requisitos.xlsx
+++ b/docs/Lista de Requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\tcc-bpmge\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F5E5E9-0F69-49E1-B489-80C54AD10F87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC86541E-E510-4F0F-A03F-C6D044457883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2B3793BC-D4C7-4BCB-9A91-426C194EAFD3}"/>
   </bookViews>
@@ -1118,154 +1118,154 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B4356-8D8F-4CB3-B9EE-8787D1D1B408}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,10 +1701,10 @@
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="103" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="67"/>
+      <c r="D11" s="104"/>
       <c r="E11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1731,10 +1731,10 @@
       <c r="B12" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="105" t="s">
         <v>160</v>
       </c>
-      <c r="D12" s="69"/>
+      <c r="D12" s="106"/>
       <c r="E12" s="23" t="s">
         <v>28</v>
       </c>
@@ -1761,10 +1761,10 @@
       <c r="B13" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="62"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="24" t="s">
         <v>28</v>
       </c>
@@ -1791,10 +1791,10 @@
       <c r="B14" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="62"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="24" t="s">
         <v>28</v>
       </c>
@@ -1821,10 +1821,10 @@
       <c r="B15" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="62"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="25" t="s">
         <v>48</v>
       </c>
@@ -1851,10 +1851,10 @@
       <c r="B16" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="61" t="s">
+      <c r="C16" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="62"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="25" t="s">
         <v>28</v>
       </c>
@@ -1881,10 +1881,10 @@
       <c r="B17" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="62"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="24" t="s">
         <v>28</v>
       </c>
@@ -1909,10 +1909,10 @@
       <c r="B18" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="62"/>
+      <c r="D18" s="67"/>
       <c r="E18" s="24" t="s">
         <v>32</v>
       </c>
@@ -1939,10 +1939,10 @@
       <c r="B19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="62"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="24" t="s">
         <v>32</v>
       </c>
@@ -1969,10 +1969,10 @@
       <c r="B20" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="62"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="24" t="s">
         <v>32</v>
       </c>
@@ -1999,10 +1999,10 @@
       <c r="B21" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="65"/>
+      <c r="D21" s="64"/>
       <c r="E21" s="25" t="s">
         <v>33</v>
       </c>
@@ -2025,8 +2025,8 @@
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="30"/>
       <c r="B22" s="31"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="71"/>
+      <c r="C22" s="107"/>
+      <c r="D22" s="108"/>
       <c r="E22" s="32"/>
       <c r="F22" s="33"/>
       <c r="G22" s="34"/>
@@ -2041,10 +2041,10 @@
       <c r="B23" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="61" t="s">
+      <c r="C23" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="62"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="24" t="s">
         <v>32</v>
       </c>
@@ -2069,10 +2069,10 @@
       <c r="B24" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="62"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="24" t="s">
         <v>32</v>
       </c>
@@ -2099,10 +2099,10 @@
       <c r="B25" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="62"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="25" t="s">
         <v>54</v>
       </c>
@@ -2129,10 +2129,10 @@
       <c r="B26" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="61" t="s">
+      <c r="C26" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="62"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="25" t="s">
         <v>54</v>
       </c>
@@ -2159,10 +2159,10 @@
       <c r="B27" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="61" t="s">
+      <c r="C27" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="D27" s="62"/>
+      <c r="D27" s="67"/>
       <c r="E27" s="24" t="s">
         <v>32</v>
       </c>
@@ -2189,10 +2189,10 @@
       <c r="B28" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="62"/>
+      <c r="D28" s="67"/>
       <c r="E28" s="25" t="s">
         <v>98</v>
       </c>
@@ -2219,10 +2219,10 @@
       <c r="B29" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="61" t="s">
+      <c r="C29" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="62"/>
+      <c r="D29" s="67"/>
       <c r="E29" s="25" t="s">
         <v>33</v>
       </c>
@@ -2247,10 +2247,10 @@
       <c r="B30" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="109" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="64"/>
+      <c r="D30" s="110"/>
       <c r="E30" s="25" t="s">
         <v>33</v>
       </c>
@@ -2275,10 +2275,10 @@
       <c r="B31" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="61" t="s">
+      <c r="C31" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="D31" s="62"/>
+      <c r="D31" s="67"/>
       <c r="E31" s="25" t="s">
         <v>107</v>
       </c>
@@ -2301,8 +2301,8 @@
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="50"/>
-      <c r="C32" s="103"/>
-      <c r="D32" s="104"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="71"/>
       <c r="E32" s="32"/>
       <c r="F32" s="45"/>
       <c r="G32" s="46"/>
@@ -2317,10 +2317,10 @@
       <c r="B33" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="61" t="s">
+      <c r="C33" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="62"/>
+      <c r="D33" s="67"/>
       <c r="E33" s="25" t="s">
         <v>33</v>
       </c>
@@ -2343,10 +2343,10 @@
       <c r="B34" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="C34" s="61" t="s">
+      <c r="C34" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="D34" s="65"/>
+      <c r="D34" s="64"/>
       <c r="E34" s="25" t="s">
         <v>111</v>
       </c>
@@ -2369,10 +2369,10 @@
       <c r="B35" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="C35" s="61" t="s">
+      <c r="C35" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="D35" s="65"/>
+      <c r="D35" s="64"/>
       <c r="E35" s="25" t="s">
         <v>111</v>
       </c>
@@ -2395,10 +2395,10 @@
       <c r="B36" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="61" t="s">
+      <c r="C36" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="D36" s="65"/>
+      <c r="D36" s="64"/>
       <c r="E36" s="25" t="s">
         <v>28</v>
       </c>
@@ -2423,10 +2423,10 @@
       <c r="B37" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="61" t="s">
+      <c r="C37" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="D37" s="65"/>
+      <c r="D37" s="64"/>
       <c r="E37" s="25" t="s">
         <v>55</v>
       </c>
@@ -2449,10 +2449,10 @@
       <c r="B38" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="61" t="s">
+      <c r="C38" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="D38" s="62"/>
+      <c r="D38" s="67"/>
       <c r="E38" s="25" t="s">
         <v>125</v>
       </c>
@@ -2475,10 +2475,10 @@
       <c r="B39" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="61" t="s">
+      <c r="C39" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="D39" s="62"/>
+      <c r="D39" s="67"/>
       <c r="E39" s="25" t="s">
         <v>57</v>
       </c>
@@ -2501,10 +2501,10 @@
       <c r="B40" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="61" t="s">
+      <c r="C40" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="62"/>
+      <c r="D40" s="67"/>
       <c r="E40" s="25" t="s">
         <v>55</v>
       </c>
@@ -2527,10 +2527,10 @@
       <c r="B41" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="C41" s="61" t="s">
+      <c r="C41" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="62"/>
+      <c r="D41" s="67"/>
       <c r="E41" s="25" t="s">
         <v>55</v>
       </c>
@@ -2549,8 +2549,8 @@
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="50"/>
-      <c r="C42" s="105"/>
-      <c r="D42" s="106"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="69"/>
       <c r="E42" s="32"/>
       <c r="F42" s="45"/>
       <c r="G42" s="46"/>
@@ -2565,8 +2565,8 @@
       <c r="B43" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="107"/>
-      <c r="D43" s="108"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="62"/>
       <c r="E43" s="25" t="s">
         <v>60</v>
       </c>
@@ -2585,8 +2585,8 @@
       <c r="B44" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="107"/>
-      <c r="D44" s="108"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="62"/>
       <c r="E44" s="25" t="s">
         <v>60</v>
       </c>
@@ -2605,8 +2605,8 @@
       <c r="B45" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="107"/>
-      <c r="D45" s="108"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="62"/>
       <c r="E45" s="25" t="s">
         <v>32</v>
       </c>
@@ -2625,8 +2625,8 @@
       <c r="B46" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="C46" s="109"/>
-      <c r="D46" s="110"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="66"/>
       <c r="E46" s="25" t="s">
         <v>28</v>
       </c>
@@ -2645,8 +2645,8 @@
       <c r="B47" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="C47" s="109"/>
-      <c r="D47" s="110"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="66"/>
       <c r="E47" s="25" t="s">
         <v>60</v>
       </c>
@@ -2665,8 +2665,8 @@
       <c r="B48" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="C48" s="109"/>
-      <c r="D48" s="110"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="66"/>
       <c r="E48" s="25" t="s">
         <v>28</v>
       </c>
@@ -2685,8 +2685,8 @@
       <c r="B49" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="C49" s="109"/>
-      <c r="D49" s="110"/>
+      <c r="C49" s="65"/>
+      <c r="D49" s="66"/>
       <c r="E49" s="25" t="s">
         <v>28</v>
       </c>
@@ -2705,10 +2705,10 @@
       <c r="B50" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="109" t="s">
+      <c r="C50" s="65" t="s">
         <v>144</v>
       </c>
-      <c r="D50" s="110"/>
+      <c r="D50" s="66"/>
       <c r="E50" s="59" t="s">
         <v>33</v>
       </c>
@@ -2727,8 +2727,8 @@
       <c r="B51" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="65"/>
+      <c r="C51" s="63"/>
+      <c r="D51" s="64"/>
       <c r="E51" s="25"/>
       <c r="F51" s="17"/>
       <c r="G51" s="10"/>
@@ -2785,8 +2785,8 @@
       <c r="B54" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="C54" s="107"/>
-      <c r="D54" s="108"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="62"/>
       <c r="E54" s="25"/>
       <c r="F54" s="17"/>
       <c r="G54" s="10"/>
@@ -2801,8 +2801,8 @@
       <c r="B55" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="C55" s="107"/>
-      <c r="D55" s="108"/>
+      <c r="C55" s="61"/>
+      <c r="D55" s="62"/>
       <c r="E55" s="25"/>
       <c r="F55" s="17"/>
       <c r="G55" s="10"/>
@@ -2817,8 +2817,8 @@
       <c r="B56" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="C56" s="107"/>
-      <c r="D56" s="108"/>
+      <c r="C56" s="61"/>
+      <c r="D56" s="62"/>
       <c r="E56" s="25"/>
       <c r="F56" s="17"/>
       <c r="G56" s="10"/>
@@ -2889,8 +2889,8 @@
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="38"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="65"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="64"/>
       <c r="E62" s="25"/>
       <c r="F62" s="17"/>
       <c r="G62" s="10"/>
@@ -2912,31 +2912,26 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C22:D22"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="I1:J2"/>
     <mergeCell ref="I5:J5"/>
@@ -2952,26 +2947,31 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C1:H2"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>